<commit_message>
Committing all the conceptual mappings v.3.3.0 for Forms F03, F06, F21, F22 and F25.
</commit_message>
<xml_diff>
--- a/mappings/package_F22/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F22/transformation/conceptual_mappings.xlsx
@@ -167,7 +167,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>3.1.1</t>
+    <t>3.2.2</t>
   </si>
   <si>
     <r>
@@ -4198,16 +4198,16 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <b/>
-      </rPr>
-      <t xml:space="preserve"> epo:specifiesSelectionCriterion / epo:epo:hasSelectionCriterionType </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-      </rPr>
-      <t>&lt;</t>
+        <b val="0"/>
+      </rPr>
+      <t xml:space="preserve"> epo:specifiesSelectionCriterion / epo:hasSelectionCriterionType</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
     </r>
     <r>
       <rPr>
@@ -4216,7 +4216,7 @@
         <color rgb="FF000000"/>
         <u/>
       </rPr>
-      <t>https://op.europa.eu/en/web/eu-vocabularies/concept/-/resource?uri=http://publications.europa.eu/resource/authority/selection-criterion/sui-act</t>
+      <t>http://publications.europa.eu/resource/authority/selection-criterion/sui-act</t>
     </r>
     <r>
       <rPr>
@@ -4254,7 +4254,7 @@
     <t>epo:Lot / epo:ContractTerm / rdf:langString</t>
   </si>
   <si>
-    <t>?this epo:foreseesContractSpecificTerm / epo:hasPerformanceConditions ?this</t>
+    <t>?this epo:foreseesContractSpecificTerm / epo:hasPerformanceConditions ?value</t>
   </si>
   <si>
     <t>III.2.3</t>
@@ -4675,7 +4675,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> epo:isSubjectToProcedureSpecificTerm  / epo:epo:hasReceiptExpressionsDeadline ?</t>
+      <t xml:space="preserve"> epo:isSubjectToProcedureSpecificTerm  / epo:hasReceiptExpressionsDeadline ?</t>
     </r>
     <r>
       <rPr>
@@ -6473,10 +6473,7 @@
     <t>Review body</t>
   </si>
   <si>
-    <t>COMPLEMENTARY_INFO</t>
-  </si>
-  <si>
-    <t>epo:ResultNotice / epo:Reviewer</t>
+    <t>COMPLEMENTARY_INFO/ADDRESS_REVIEW_BODY</t>
   </si>
   <si>
     <t>VI.4.1.1</t>
@@ -6761,6 +6758,9 @@
     <t>Body responsible for mediation procedures</t>
   </si>
   <si>
+    <t>COMPLEMENTARY_INFO/ADDRESS_MEDIATION_BODY</t>
+  </si>
+  <si>
     <t>epo:ResultNotice / epo:Mediator</t>
   </si>
   <si>
@@ -7054,7 +7054,7 @@
     <t>Service from which information about the review procedure may be obtained</t>
   </si>
   <si>
-    <t>epo:ResultNotice / epo:ReviewProcedureInformationProvider</t>
+    <t>COMPLEMENTARY_INFO/ADDRESS_REVIEW_INFO</t>
   </si>
   <si>
     <t>VI.4.4.1</t>
@@ -8151,7 +8151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8258,11 +8258,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -8559,7 +8554,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="201">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8852,6 +8847,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="8" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -8869,9 +8867,6 @@
     </xf>
     <xf borderId="0" fillId="16" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -8937,7 +8932,7 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -8945,13 +8940,10 @@
     <xf borderId="0" fillId="9" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -8960,10 +8952,10 @@
     <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -8972,7 +8964,7 @@
     <xf borderId="0" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -8993,10 +8985,10 @@
     <xf borderId="0" fillId="6" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9011,13 +9003,13 @@
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="6" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="6" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -9053,13 +9045,13 @@
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9077,13 +9069,13 @@
     <xf quotePrefix="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9099,16 +9091,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9135,7 +9127,7 @@
     <xf borderId="0" fillId="18" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="10" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -9147,13 +9139,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -15918,17 +15910,17 @@
       <c r="C108" s="64" t="s">
         <v>470</v>
       </c>
-      <c r="D108" s="57" t="s">
+      <c r="D108" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="E108" s="81" t="s">
+      <c r="E108" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="F108" s="57"/>
-      <c r="G108" s="81" t="s">
+      <c r="F108" s="4"/>
+      <c r="G108" s="100" t="s">
         <v>472</v>
       </c>
-      <c r="H108" s="57" t="s">
+      <c r="H108" s="42" t="s">
         <v>473</v>
       </c>
       <c r="I108" s="7"/>
@@ -15945,15 +15937,15 @@
       <c r="C109" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="D109" s="57"/>
-      <c r="E109" s="81" t="s">
+      <c r="D109" s="4"/>
+      <c r="E109" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="F109" s="57"/>
-      <c r="G109" s="81" t="s">
+      <c r="F109" s="4"/>
+      <c r="G109" s="100" t="s">
         <v>476</v>
       </c>
-      <c r="H109" s="81" t="s">
+      <c r="H109" s="100" t="s">
         <v>477</v>
       </c>
       <c r="I109" s="7"/>
@@ -15964,11 +15956,11 @@
       <c r="A110" s="48" t="s">
         <v>478</v>
       </c>
-      <c r="B110" s="100" t="s">
+      <c r="B110" s="101" t="s">
         <v>479</v>
       </c>
-      <c r="C110" s="101"/>
-      <c r="D110" s="101"/>
+      <c r="C110" s="102"/>
+      <c r="D110" s="102"/>
       <c r="E110" s="64"/>
       <c r="F110" s="64"/>
       <c r="G110" s="64"/>
@@ -15984,7 +15976,7 @@
       <c r="B111" s="57" t="s">
         <v>481</v>
       </c>
-      <c r="C111" s="102" t="s">
+      <c r="C111" s="103" t="s">
         <v>482</v>
       </c>
       <c r="D111" s="85" t="s">
@@ -16005,11 +15997,11 @@
       <c r="K111" s="87"/>
     </row>
     <row r="112">
-      <c r="A112" s="103" t="s">
+      <c r="A112" s="104" t="s">
         <v>487</v>
       </c>
-      <c r="B112" s="104"/>
-      <c r="C112" s="102"/>
+      <c r="B112" s="105"/>
+      <c r="C112" s="103"/>
       <c r="D112" s="85"/>
       <c r="E112" s="85" t="s">
         <v>488</v>
@@ -16028,11 +16020,11 @@
       <c r="K112" s="87"/>
     </row>
     <row r="113">
-      <c r="A113" s="103" t="s">
+      <c r="A113" s="104" t="s">
         <v>487</v>
       </c>
-      <c r="B113" s="104"/>
-      <c r="C113" s="105"/>
+      <c r="B113" s="105"/>
+      <c r="C113" s="106"/>
       <c r="D113" s="87"/>
       <c r="E113" s="85" t="s">
         <v>488</v>
@@ -16057,7 +16049,7 @@
       <c r="B114" s="57" t="s">
         <v>495</v>
       </c>
-      <c r="C114" s="102" t="s">
+      <c r="C114" s="103" t="s">
         <v>496</v>
       </c>
       <c r="D114" s="85" t="s">
@@ -16084,7 +16076,7 @@
       <c r="B115" s="57" t="s">
         <v>502</v>
       </c>
-      <c r="C115" s="102" t="s">
+      <c r="C115" s="103" t="s">
         <v>503</v>
       </c>
       <c r="D115" s="85" t="s">
@@ -16164,7 +16156,7 @@
       <c r="G118" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="H118" s="106" t="s">
+      <c r="H118" s="100" t="s">
         <v>517</v>
       </c>
       <c r="I118" s="7"/>
@@ -16189,7 +16181,7 @@
       <c r="G119" s="107" t="s">
         <v>516</v>
       </c>
-      <c r="H119" s="106" t="s">
+      <c r="H119" s="100" t="s">
         <v>520</v>
       </c>
       <c r="I119" s="7"/>
@@ -16209,8 +16201,8 @@
         <v>523</v>
       </c>
       <c r="F120" s="4"/>
-      <c r="G120" s="106"/>
-      <c r="H120" s="106"/>
+      <c r="G120" s="100"/>
+      <c r="H120" s="100"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7" t="s">
@@ -16571,10 +16563,10 @@
         <v>590</v>
       </c>
       <c r="F136" s="4"/>
-      <c r="G136" s="106" t="s">
+      <c r="G136" s="100" t="s">
         <v>564</v>
       </c>
-      <c r="H136" s="106" t="s">
+      <c r="H136" s="100" t="s">
         <v>591</v>
       </c>
       <c r="I136" s="7"/>
@@ -16594,10 +16586,10 @@
         <v>594</v>
       </c>
       <c r="F137" s="4"/>
-      <c r="G137" s="106" t="s">
+      <c r="G137" s="100" t="s">
         <v>564</v>
       </c>
-      <c r="H137" s="106" t="s">
+      <c r="H137" s="100" t="s">
         <v>565</v>
       </c>
       <c r="I137" s="7"/>
@@ -16655,7 +16647,7 @@
       <c r="F140" s="64" t="s">
         <v>572</v>
       </c>
-      <c r="G140" s="106" t="s">
+      <c r="G140" s="100" t="s">
         <v>603</v>
       </c>
       <c r="H140" s="127" t="s">
@@ -16680,10 +16672,10 @@
         <v>608</v>
       </c>
       <c r="F141" s="64"/>
-      <c r="G141" s="106" t="s">
+      <c r="G141" s="100" t="s">
         <v>564</v>
       </c>
-      <c r="H141" s="106" t="s">
+      <c r="H141" s="100" t="s">
         <v>565</v>
       </c>
       <c r="I141" s="7"/>
@@ -16705,7 +16697,7 @@
         <v>612</v>
       </c>
       <c r="F142" s="64"/>
-      <c r="G142" s="106" t="s">
+      <c r="G142" s="100" t="s">
         <v>613</v>
       </c>
       <c r="H142" s="128" t="s">
@@ -16749,10 +16741,10 @@
       <c r="F144" s="68" t="s">
         <v>572</v>
       </c>
-      <c r="G144" s="106" t="s">
+      <c r="G144" s="100" t="s">
         <v>621</v>
       </c>
-      <c r="H144" s="130" t="s">
+      <c r="H144" s="128" t="s">
         <v>622</v>
       </c>
       <c r="I144" s="7"/>
@@ -16776,10 +16768,10 @@
       <c r="F145" s="64" t="s">
         <v>623</v>
       </c>
-      <c r="G145" s="106" t="s">
+      <c r="G145" s="100" t="s">
         <v>621</v>
       </c>
-      <c r="H145" s="131" t="s">
+      <c r="H145" s="130" t="s">
         <v>624</v>
       </c>
       <c r="I145" s="7"/>
@@ -16787,7 +16779,7 @@
       <c r="K145" s="7"/>
     </row>
     <row r="146">
-      <c r="A146" s="132" t="s">
+      <c r="A146" s="131" t="s">
         <v>625</v>
       </c>
       <c r="B146" s="83" t="s">
@@ -16842,7 +16834,7 @@
       <c r="G148" s="37" t="s">
         <v>635</v>
       </c>
-      <c r="H148" s="133" t="s">
+      <c r="H148" s="132" t="s">
         <v>636</v>
       </c>
       <c r="I148" s="7"/>
@@ -16869,7 +16861,7 @@
       <c r="G149" s="37" t="s">
         <v>635</v>
       </c>
-      <c r="H149" s="133" t="s">
+      <c r="H149" s="132" t="s">
         <v>640</v>
       </c>
       <c r="I149" s="7"/>
@@ -16923,7 +16915,7 @@
       <c r="G151" s="37" t="s">
         <v>635</v>
       </c>
-      <c r="H151" s="133" t="s">
+      <c r="H151" s="132" t="s">
         <v>648</v>
       </c>
       <c r="I151" s="7"/>
@@ -16989,7 +16981,7 @@
         <v>661</v>
       </c>
       <c r="F154" s="51"/>
-      <c r="G154" s="106" t="s">
+      <c r="G154" s="100" t="s">
         <v>662</v>
       </c>
       <c r="H154" s="42" t="s">
@@ -17023,7 +17015,7 @@
       <c r="B156" s="57" t="s">
         <v>667</v>
       </c>
-      <c r="C156" s="134" t="s">
+      <c r="C156" s="133" t="s">
         <v>226</v>
       </c>
       <c r="D156" s="68"/>
@@ -17031,7 +17023,7 @@
         <v>668</v>
       </c>
       <c r="F156" s="4"/>
-      <c r="G156" s="106" t="s">
+      <c r="G156" s="100" t="s">
         <v>669</v>
       </c>
       <c r="H156" s="109" t="s">
@@ -17080,11 +17072,11 @@
       <c r="E158" s="64" t="s">
         <v>678</v>
       </c>
-      <c r="F158" s="106"/>
+      <c r="F158" s="100"/>
       <c r="G158" s="64" t="s">
         <v>679</v>
       </c>
-      <c r="H158" s="135" t="s">
+      <c r="H158" s="134" t="s">
         <v>680</v>
       </c>
       <c r="I158" s="7"/>
@@ -17105,11 +17097,11 @@
       <c r="E159" s="64" t="s">
         <v>684</v>
       </c>
-      <c r="F159" s="106"/>
-      <c r="G159" s="106" t="s">
+      <c r="F159" s="100"/>
+      <c r="G159" s="100" t="s">
         <v>679</v>
       </c>
-      <c r="H159" s="135" t="s">
+      <c r="H159" s="134" t="s">
         <v>685</v>
       </c>
       <c r="I159" s="7"/>
@@ -17134,7 +17126,7 @@
       <c r="G160" s="64" t="s">
         <v>690</v>
       </c>
-      <c r="H160" s="135" t="s">
+      <c r="H160" s="134" t="s">
         <v>691</v>
       </c>
       <c r="I160" s="7"/>
@@ -17157,7 +17149,7 @@
       </c>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
-      <c r="H161" s="106"/>
+      <c r="H161" s="100"/>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
       <c r="K161" s="7"/>
@@ -17199,7 +17191,7 @@
       <c r="G163" s="37" t="s">
         <v>702</v>
       </c>
-      <c r="H163" s="136" t="s">
+      <c r="H163" s="135" t="s">
         <v>703</v>
       </c>
       <c r="I163" s="7"/>
@@ -17207,7 +17199,7 @@
       <c r="K163" s="7"/>
     </row>
     <row r="164">
-      <c r="A164" s="132" t="s">
+      <c r="A164" s="131" t="s">
         <v>704</v>
       </c>
       <c r="B164" s="35" t="s">
@@ -17224,7 +17216,7 @@
       <c r="G164" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="H164" s="137" t="s">
+      <c r="H164" s="136" t="s">
         <v>709</v>
       </c>
       <c r="I164" s="7"/>
@@ -17232,10 +17224,10 @@
       <c r="K164" s="7"/>
     </row>
     <row r="165">
-      <c r="A165" s="138" t="s">
+      <c r="A165" s="137" t="s">
         <v>704</v>
       </c>
-      <c r="B165" s="139" t="s">
+      <c r="B165" s="138" t="s">
         <v>705</v>
       </c>
       <c r="C165" s="63"/>
@@ -17249,7 +17241,7 @@
       <c r="G165" s="66" t="s">
         <v>710</v>
       </c>
-      <c r="H165" s="140" t="s">
+      <c r="H165" s="139" t="s">
         <v>711</v>
       </c>
       <c r="I165" s="7"/>
@@ -17257,10 +17249,10 @@
       <c r="K165" s="7"/>
     </row>
     <row r="166">
-      <c r="A166" s="138" t="s">
+      <c r="A166" s="137" t="s">
         <v>704</v>
       </c>
-      <c r="B166" s="139" t="s">
+      <c r="B166" s="138" t="s">
         <v>705</v>
       </c>
       <c r="C166" s="63"/>
@@ -17365,10 +17357,10 @@
       <c r="K169" s="7"/>
     </row>
     <row r="170">
-      <c r="A170" s="141" t="s">
+      <c r="A170" s="140" t="s">
         <v>727</v>
       </c>
-      <c r="B170" s="142" t="s">
+      <c r="B170" s="141" t="s">
         <v>728</v>
       </c>
       <c r="C170" s="114" t="s">
@@ -17392,13 +17384,13 @@
       <c r="K170" s="7"/>
     </row>
     <row r="171">
-      <c r="A171" s="143" t="s">
+      <c r="A171" s="142" t="s">
         <v>737</v>
       </c>
       <c r="B171" s="40" t="s">
         <v>738</v>
       </c>
-      <c r="C171" s="144" t="s">
+      <c r="C171" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D171" s="63"/>
@@ -17417,12 +17409,12 @@
       <c r="B172" s="49" t="s">
         <v>741</v>
       </c>
-      <c r="C172" s="144" t="s">
+      <c r="C172" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D172" s="37"/>
-      <c r="E172" s="145"/>
-      <c r="F172" s="145"/>
+      <c r="E172" s="144"/>
+      <c r="F172" s="144"/>
       <c r="G172" s="37"/>
       <c r="H172" s="37"/>
       <c r="I172" s="7"/>
@@ -17442,14 +17434,14 @@
       <c r="D173" s="63" t="s">
         <v>745</v>
       </c>
-      <c r="E173" s="146" t="s">
+      <c r="E173" s="145" t="s">
         <v>746</v>
       </c>
-      <c r="F173" s="146"/>
+      <c r="F173" s="145"/>
       <c r="G173" s="63" t="s">
         <v>747</v>
       </c>
-      <c r="H173" s="147" t="s">
+      <c r="H173" s="146" t="s">
         <v>748</v>
       </c>
       <c r="I173" s="7"/>
@@ -17476,7 +17468,7 @@
       <c r="G174" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="H174" s="148" t="s">
+      <c r="H174" s="147" t="s">
         <v>752</v>
       </c>
       <c r="I174" s="7"/>
@@ -17490,7 +17482,7 @@
       <c r="B175" s="57" t="s">
         <v>754</v>
       </c>
-      <c r="C175" s="149" t="s">
+      <c r="C175" s="148" t="s">
         <v>607</v>
       </c>
       <c r="D175" s="63"/>
@@ -17509,13 +17501,13 @@
       <c r="K175" s="7"/>
     </row>
     <row r="176">
-      <c r="A176" s="143" t="s">
+      <c r="A176" s="142" t="s">
         <v>758</v>
       </c>
       <c r="B176" s="40" t="s">
         <v>705</v>
       </c>
-      <c r="C176" s="144" t="s">
+      <c r="C176" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D176" s="63"/>
@@ -17603,12 +17595,12 @@
       <c r="B180" s="49" t="s">
         <v>771</v>
       </c>
-      <c r="C180" s="150"/>
-      <c r="D180" s="151"/>
+      <c r="C180" s="149"/>
+      <c r="D180" s="150"/>
       <c r="E180" s="42" t="s">
         <v>731</v>
       </c>
-      <c r="F180" s="150"/>
+      <c r="F180" s="149"/>
       <c r="G180" s="51" t="s">
         <v>772</v>
       </c>
@@ -17685,7 +17677,7 @@
       <c r="G183" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="H183" s="148" t="s">
+      <c r="H183" s="147" t="s">
         <v>789</v>
       </c>
       <c r="I183" s="7"/>
@@ -17745,7 +17737,7 @@
       <c r="B186" s="57" t="s">
         <v>799</v>
       </c>
-      <c r="C186" s="152" t="s">
+      <c r="C186" s="151" t="s">
         <v>800</v>
       </c>
       <c r="D186" s="63"/>
@@ -17770,7 +17762,7 @@
       <c r="B187" s="49" t="s">
         <v>803</v>
       </c>
-      <c r="C187" s="144" t="s">
+      <c r="C187" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D187" s="63"/>
@@ -17966,7 +17958,7 @@
       <c r="G194" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="H194" s="153" t="s">
+      <c r="H194" s="152" t="s">
         <v>826</v>
       </c>
       <c r="I194" s="7"/>
@@ -18047,7 +18039,7 @@
       <c r="G197" s="47" t="s">
         <v>829</v>
       </c>
-      <c r="H197" s="154" t="s">
+      <c r="H197" s="153" t="s">
         <v>838</v>
       </c>
       <c r="I197" s="7"/>
@@ -18101,7 +18093,7 @@
       <c r="G199" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="H199" s="155" t="s">
+      <c r="H199" s="154" t="s">
         <v>848</v>
       </c>
       <c r="I199" s="7"/>
@@ -18109,7 +18101,7 @@
       <c r="K199" s="7"/>
     </row>
     <row r="200">
-      <c r="A200" s="156"/>
+      <c r="A200" s="155"/>
       <c r="B200" s="4"/>
       <c r="C200" s="63"/>
       <c r="D200" s="63"/>
@@ -18134,7 +18126,7 @@
       <c r="B201" s="49" t="s">
         <v>852</v>
       </c>
-      <c r="C201" s="157" t="s">
+      <c r="C201" s="156" t="s">
         <v>739</v>
       </c>
       <c r="D201" s="63"/>
@@ -18174,13 +18166,13 @@
       <c r="K202" s="7"/>
     </row>
     <row r="203">
-      <c r="A203" s="103" t="s">
+      <c r="A203" s="104" t="s">
         <v>857</v>
       </c>
       <c r="B203" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C203" s="158" t="s">
+      <c r="C203" s="157" t="s">
         <v>226</v>
       </c>
       <c r="D203" s="63"/>
@@ -18226,16 +18218,16 @@
       <c r="K204" s="7"/>
     </row>
     <row r="205">
-      <c r="A205" s="103" t="s">
+      <c r="A205" s="104" t="s">
         <v>868</v>
       </c>
       <c r="B205" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C205" s="159" t="s">
+      <c r="C205" s="158" t="s">
         <v>226</v>
       </c>
-      <c r="D205" s="160"/>
+      <c r="D205" s="159"/>
       <c r="E205" s="51" t="s">
         <v>869</v>
       </c>
@@ -18278,13 +18270,13 @@
       <c r="K206" s="7"/>
     </row>
     <row r="207">
-      <c r="A207" s="103" t="s">
+      <c r="A207" s="104" t="s">
         <v>876</v>
       </c>
       <c r="B207" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C207" s="158" t="s">
+      <c r="C207" s="157" t="s">
         <v>226</v>
       </c>
       <c r="D207" s="63"/>
@@ -18330,13 +18322,13 @@
       <c r="K208" s="7"/>
     </row>
     <row r="209">
-      <c r="A209" s="103" t="s">
+      <c r="A209" s="104" t="s">
         <v>883</v>
       </c>
       <c r="B209" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="C209" s="158" t="s">
+      <c r="C209" s="157" t="s">
         <v>226</v>
       </c>
       <c r="D209" s="63"/>
@@ -18361,7 +18353,7 @@
       <c r="B210" s="49" t="s">
         <v>886</v>
       </c>
-      <c r="C210" s="144" t="s">
+      <c r="C210" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D210" s="63"/>
@@ -18451,14 +18443,14 @@
       <c r="B214" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="C214" s="158" t="s">
+      <c r="C214" s="157" t="s">
         <v>226</v>
       </c>
       <c r="D214" s="63"/>
-      <c r="E214" s="146" t="s">
+      <c r="E214" s="145" t="s">
         <v>903</v>
       </c>
-      <c r="F214" s="146"/>
+      <c r="F214" s="145"/>
       <c r="G214" s="51" t="s">
         <v>904</v>
       </c>
@@ -18476,16 +18468,16 @@
       <c r="B215" s="57" t="s">
         <v>907</v>
       </c>
-      <c r="C215" s="145" t="s">
+      <c r="C215" s="144" t="s">
         <v>908</v>
       </c>
-      <c r="D215" s="145" t="s">
+      <c r="D215" s="144" t="s">
         <v>909</v>
       </c>
-      <c r="E215" s="146" t="s">
+      <c r="E215" s="145" t="s">
         <v>910</v>
       </c>
-      <c r="F215" s="146"/>
+      <c r="F215" s="145"/>
       <c r="G215" s="51" t="s">
         <v>911</v>
       </c>
@@ -18503,16 +18495,16 @@
       <c r="B216" s="57" t="s">
         <v>914</v>
       </c>
-      <c r="C216" s="145" t="s">
+      <c r="C216" s="144" t="s">
         <v>915</v>
       </c>
-      <c r="D216" s="145" t="s">
+      <c r="D216" s="144" t="s">
         <v>916</v>
       </c>
-      <c r="E216" s="146" t="s">
+      <c r="E216" s="145" t="s">
         <v>917</v>
       </c>
-      <c r="F216" s="146"/>
+      <c r="F216" s="145"/>
       <c r="G216" s="51" t="s">
         <v>918</v>
       </c>
@@ -18530,10 +18522,10 @@
       <c r="B217" s="40" t="s">
         <v>921</v>
       </c>
-      <c r="C217" s="161"/>
-      <c r="D217" s="161"/>
-      <c r="E217" s="161"/>
-      <c r="F217" s="145"/>
+      <c r="C217" s="160"/>
+      <c r="D217" s="160"/>
+      <c r="E217" s="160"/>
+      <c r="F217" s="144"/>
       <c r="G217" s="51"/>
       <c r="H217" s="51"/>
       <c r="I217" s="7"/>
@@ -18547,15 +18539,15 @@
       <c r="B218" s="49" t="s">
         <v>923</v>
       </c>
-      <c r="C218" s="161" t="s">
+      <c r="C218" s="160" t="s">
         <v>924</v>
       </c>
-      <c r="D218" s="161"/>
-      <c r="E218" s="161" t="s">
+      <c r="D218" s="160"/>
+      <c r="E218" s="160" t="s">
         <v>925</v>
       </c>
-      <c r="F218" s="145"/>
-      <c r="G218" s="106" t="s">
+      <c r="F218" s="144"/>
+      <c r="G218" s="100" t="s">
         <v>926</v>
       </c>
       <c r="H218" s="109" t="s">
@@ -18572,15 +18564,15 @@
       <c r="B219" s="49" t="s">
         <v>929</v>
       </c>
-      <c r="C219" s="161" t="s">
+      <c r="C219" s="160" t="s">
         <v>930</v>
       </c>
-      <c r="D219" s="161"/>
-      <c r="E219" s="161" t="s">
+      <c r="D219" s="160"/>
+      <c r="E219" s="160" t="s">
         <v>931</v>
       </c>
-      <c r="F219" s="145"/>
-      <c r="G219" s="106" t="s">
+      <c r="F219" s="144"/>
+      <c r="G219" s="100" t="s">
         <v>926</v>
       </c>
       <c r="H219" s="109" t="s">
@@ -18597,15 +18589,15 @@
       <c r="B220" s="49" t="s">
         <v>934</v>
       </c>
-      <c r="C220" s="161" t="s">
+      <c r="C220" s="160" t="s">
         <v>935</v>
       </c>
-      <c r="D220" s="161"/>
-      <c r="E220" s="161" t="s">
+      <c r="D220" s="160"/>
+      <c r="E220" s="160" t="s">
         <v>936</v>
       </c>
-      <c r="F220" s="145"/>
-      <c r="G220" s="106" t="s">
+      <c r="F220" s="144"/>
+      <c r="G220" s="100" t="s">
         <v>926</v>
       </c>
       <c r="H220" s="109" t="s">
@@ -18616,7 +18608,7 @@
       <c r="K220" s="7"/>
     </row>
     <row r="221">
-      <c r="A221" s="143" t="s">
+      <c r="A221" s="142" t="s">
         <v>938</v>
       </c>
       <c r="B221" s="40" t="s">
@@ -18628,14 +18620,14 @@
       <c r="D221" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="E221" s="146" t="s">
+      <c r="E221" s="145" t="s">
         <v>939</v>
       </c>
-      <c r="F221" s="146"/>
-      <c r="G221" s="162" t="s">
+      <c r="F221" s="145"/>
+      <c r="G221" s="161" t="s">
         <v>309</v>
       </c>
-      <c r="H221" s="163" t="s">
+      <c r="H221" s="162" t="s">
         <v>940</v>
       </c>
       <c r="I221" s="7"/>
@@ -18643,18 +18635,18 @@
       <c r="K221" s="7"/>
     </row>
     <row r="222">
-      <c r="A222" s="143" t="s">
+      <c r="A222" s="142" t="s">
         <v>941</v>
       </c>
       <c r="B222" s="62" t="s">
         <v>942</v>
       </c>
-      <c r="C222" s="144" t="s">
+      <c r="C222" s="143" t="s">
         <v>739</v>
       </c>
       <c r="D222" s="7"/>
-      <c r="E222" s="145"/>
-      <c r="F222" s="145"/>
+      <c r="E222" s="144"/>
+      <c r="F222" s="144"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="7"/>
@@ -18668,16 +18660,16 @@
       <c r="B223" s="67" t="s">
         <v>944</v>
       </c>
-      <c r="C223" s="164" t="s">
+      <c r="C223" s="163" t="s">
         <v>739</v>
       </c>
       <c r="D223" s="7"/>
       <c r="E223" s="41" t="s">
         <v>945</v>
       </c>
-      <c r="F223" s="63"/>
+      <c r="F223" s="66"/>
       <c r="G223" s="37" t="s">
-        <v>946</v>
+        <v>53</v>
       </c>
       <c r="H223" s="37" t="s">
         <v>231</v>
@@ -18688,9 +18680,9 @@
     </row>
     <row r="224">
       <c r="A224" s="86" t="s">
-        <v>947</v>
-      </c>
-      <c r="B224" s="165" t="s">
+        <v>946</v>
+      </c>
+      <c r="B224" s="164" t="s">
         <v>56</v>
       </c>
       <c r="C224" s="63" t="s">
@@ -18700,14 +18692,14 @@
         <v>58</v>
       </c>
       <c r="E224" s="66" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F224" s="66"/>
       <c r="G224" s="84" t="s">
         <v>60</v>
       </c>
       <c r="H224" s="84" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
@@ -18715,9 +18707,9 @@
     </row>
     <row r="225">
       <c r="A225" s="86" t="s">
-        <v>950</v>
-      </c>
-      <c r="B225" s="165" t="s">
+        <v>949</v>
+      </c>
+      <c r="B225" s="164" t="s">
         <v>70</v>
       </c>
       <c r="C225" s="63" t="s">
@@ -18727,14 +18719,14 @@
         <v>72</v>
       </c>
       <c r="E225" s="51" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F225" s="66"/>
       <c r="G225" s="41" t="s">
         <v>74</v>
       </c>
       <c r="H225" s="41" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I225" s="7"/>
       <c r="J225" s="7"/>
@@ -18742,9 +18734,9 @@
     </row>
     <row r="226">
       <c r="A226" s="86" t="s">
-        <v>953</v>
-      </c>
-      <c r="B226" s="165" t="s">
+        <v>952</v>
+      </c>
+      <c r="B226" s="164" t="s">
         <v>77</v>
       </c>
       <c r="C226" s="63" t="s">
@@ -18754,14 +18746,14 @@
         <v>79</v>
       </c>
       <c r="E226" s="66" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F226" s="66"/>
       <c r="G226" s="84" t="s">
         <v>74</v>
       </c>
       <c r="H226" s="84" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I226" s="7"/>
       <c r="J226" s="7"/>
@@ -18769,9 +18761,9 @@
     </row>
     <row r="227">
       <c r="A227" s="86" t="s">
-        <v>956</v>
-      </c>
-      <c r="B227" s="165" t="s">
+        <v>955</v>
+      </c>
+      <c r="B227" s="164" t="s">
         <v>91</v>
       </c>
       <c r="C227" s="63" t="s">
@@ -18781,14 +18773,14 @@
         <v>821</v>
       </c>
       <c r="E227" s="51" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F227" s="66"/>
       <c r="G227" s="41" t="s">
+        <v>957</v>
+      </c>
+      <c r="H227" s="41" t="s">
         <v>958</v>
-      </c>
-      <c r="H227" s="41" t="s">
-        <v>959</v>
       </c>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
@@ -18796,9 +18788,9 @@
     </row>
     <row r="228">
       <c r="A228" s="86" t="s">
-        <v>960</v>
-      </c>
-      <c r="B228" s="165" t="s">
+        <v>959</v>
+      </c>
+      <c r="B228" s="164" t="s">
         <v>98</v>
       </c>
       <c r="C228" s="63" t="s">
@@ -18808,14 +18800,14 @@
         <v>100</v>
       </c>
       <c r="E228" s="66" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F228" s="66"/>
       <c r="G228" s="66" t="s">
         <v>102</v>
       </c>
       <c r="H228" s="66" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
@@ -18823,9 +18815,9 @@
     </row>
     <row r="229">
       <c r="A229" s="86" t="s">
-        <v>963</v>
-      </c>
-      <c r="B229" s="165" t="s">
+        <v>962</v>
+      </c>
+      <c r="B229" s="164" t="s">
         <v>118</v>
       </c>
       <c r="C229" s="66" t="s">
@@ -18835,7 +18827,7 @@
         <v>120</v>
       </c>
       <c r="E229" s="66" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F229" s="66"/>
       <c r="G229" s="66" t="s">
@@ -18850,9 +18842,9 @@
     </row>
     <row r="230">
       <c r="A230" s="86" t="s">
-        <v>965</v>
-      </c>
-      <c r="B230" s="165" t="s">
+        <v>964</v>
+      </c>
+      <c r="B230" s="164" t="s">
         <v>112</v>
       </c>
       <c r="C230" s="63" t="s">
@@ -18861,10 +18853,10 @@
       <c r="D230" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="E230" s="146" t="s">
-        <v>966</v>
-      </c>
-      <c r="F230" s="146"/>
+      <c r="E230" s="145" t="s">
+        <v>965</v>
+      </c>
+      <c r="F230" s="145"/>
       <c r="G230" s="66" t="s">
         <v>833</v>
       </c>
@@ -18877,9 +18869,9 @@
     </row>
     <row r="231">
       <c r="A231" s="86" t="s">
-        <v>967</v>
-      </c>
-      <c r="B231" s="165" t="s">
+        <v>966</v>
+      </c>
+      <c r="B231" s="164" t="s">
         <v>836</v>
       </c>
       <c r="C231" s="63" t="s">
@@ -18888,15 +18880,15 @@
       <c r="D231" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="E231" s="146" t="s">
-        <v>968</v>
-      </c>
-      <c r="F231" s="146"/>
+      <c r="E231" s="145" t="s">
+        <v>967</v>
+      </c>
+      <c r="F231" s="145"/>
       <c r="G231" s="47" t="s">
         <v>829</v>
       </c>
       <c r="H231" s="47" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I231" s="7"/>
       <c r="J231" s="7"/>
@@ -18904,9 +18896,9 @@
     </row>
     <row r="232">
       <c r="A232" s="86" t="s">
-        <v>970</v>
-      </c>
-      <c r="B232" s="165" t="s">
+        <v>969</v>
+      </c>
+      <c r="B232" s="164" t="s">
         <v>125</v>
       </c>
       <c r="C232" s="63" t="s">
@@ -18915,10 +18907,10 @@
       <c r="D232" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="E232" s="146" t="s">
-        <v>971</v>
-      </c>
-      <c r="F232" s="146"/>
+      <c r="E232" s="145" t="s">
+        <v>970</v>
+      </c>
+      <c r="F232" s="145"/>
       <c r="G232" s="51" t="s">
         <v>833</v>
       </c>
@@ -18931,19 +18923,19 @@
     </row>
     <row r="233">
       <c r="A233" s="50" t="s">
+        <v>971</v>
+      </c>
+      <c r="B233" s="67" t="s">
         <v>972</v>
       </c>
-      <c r="B233" s="67" t="s">
+      <c r="C233" s="163" t="s">
+        <v>739</v>
+      </c>
+      <c r="D233" s="165"/>
+      <c r="E233" s="79" t="s">
         <v>973</v>
       </c>
-      <c r="C233" s="164" t="s">
-        <v>739</v>
-      </c>
-      <c r="D233" s="166"/>
-      <c r="E233" s="79" t="s">
-        <v>945</v>
-      </c>
-      <c r="F233" s="145"/>
+      <c r="F233" s="144"/>
       <c r="G233" s="37" t="s">
         <v>974</v>
       </c>
@@ -18958,7 +18950,7 @@
       <c r="A234" s="86" t="s">
         <v>975</v>
       </c>
-      <c r="B234" s="165" t="s">
+      <c r="B234" s="164" t="s">
         <v>56</v>
       </c>
       <c r="C234" s="63" t="s">
@@ -18967,14 +18959,14 @@
       <c r="D234" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E234" s="146" t="s">
+      <c r="E234" s="145" t="s">
         <v>976</v>
       </c>
-      <c r="F234" s="146"/>
+      <c r="F234" s="145"/>
       <c r="G234" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="H234" s="167" t="s">
+      <c r="H234" s="166" t="s">
         <v>977</v>
       </c>
       <c r="I234" s="7"/>
@@ -18985,7 +18977,7 @@
       <c r="A235" s="86" t="s">
         <v>978</v>
       </c>
-      <c r="B235" s="165" t="s">
+      <c r="B235" s="164" t="s">
         <v>70</v>
       </c>
       <c r="C235" s="63" t="s">
@@ -18994,14 +18986,14 @@
       <c r="D235" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="E235" s="146" t="s">
+      <c r="E235" s="145" t="s">
         <v>979</v>
       </c>
-      <c r="F235" s="146"/>
+      <c r="F235" s="145"/>
       <c r="G235" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H235" s="167" t="s">
+      <c r="H235" s="166" t="s">
         <v>980</v>
       </c>
       <c r="I235" s="7"/>
@@ -19012,7 +19004,7 @@
       <c r="A236" s="86" t="s">
         <v>981</v>
       </c>
-      <c r="B236" s="165" t="s">
+      <c r="B236" s="164" t="s">
         <v>77</v>
       </c>
       <c r="C236" s="63" t="s">
@@ -19039,7 +19031,7 @@
       <c r="A237" s="86" t="s">
         <v>984</v>
       </c>
-      <c r="B237" s="165" t="s">
+      <c r="B237" s="164" t="s">
         <v>91</v>
       </c>
       <c r="C237" s="63" t="s">
@@ -19066,7 +19058,7 @@
       <c r="A238" s="86" t="s">
         <v>987</v>
       </c>
-      <c r="B238" s="165" t="s">
+      <c r="B238" s="164" t="s">
         <v>98</v>
       </c>
       <c r="C238" s="63" t="s">
@@ -19093,7 +19085,7 @@
       <c r="A239" s="86" t="s">
         <v>990</v>
       </c>
-      <c r="B239" s="165" t="s">
+      <c r="B239" s="164" t="s">
         <v>118</v>
       </c>
       <c r="C239" s="66" t="s">
@@ -19120,7 +19112,7 @@
       <c r="A240" s="86" t="s">
         <v>992</v>
       </c>
-      <c r="B240" s="165" t="s">
+      <c r="B240" s="164" t="s">
         <v>112</v>
       </c>
       <c r="C240" s="63" t="s">
@@ -19147,7 +19139,7 @@
       <c r="A241" s="86" t="s">
         <v>994</v>
       </c>
-      <c r="B241" s="165" t="s">
+      <c r="B241" s="164" t="s">
         <v>836</v>
       </c>
       <c r="C241" s="63" t="s">
@@ -19174,7 +19166,7 @@
       <c r="A242" s="86" t="s">
         <v>997</v>
       </c>
-      <c r="B242" s="165" t="s">
+      <c r="B242" s="164" t="s">
         <v>125</v>
       </c>
       <c r="C242" s="63" t="s">
@@ -19214,10 +19206,10 @@
         <v>1003</v>
       </c>
       <c r="F243" s="66"/>
-      <c r="G243" s="162" t="s">
+      <c r="G243" s="161" t="s">
         <v>1004</v>
       </c>
-      <c r="H243" s="163" t="s">
+      <c r="H243" s="162" t="s">
         <v>1005</v>
       </c>
       <c r="I243" s="7"/>
@@ -19234,11 +19226,11 @@
       <c r="C244" s="7"/>
       <c r="D244" s="7"/>
       <c r="E244" s="84" t="s">
-        <v>945</v>
+        <v>1008</v>
       </c>
       <c r="F244" s="63"/>
       <c r="G244" s="63" t="s">
-        <v>1008</v>
+        <v>53</v>
       </c>
       <c r="H244" s="63" t="s">
         <v>231</v>
@@ -19251,7 +19243,7 @@
       <c r="A245" s="86" t="s">
         <v>1009</v>
       </c>
-      <c r="B245" s="165" t="s">
+      <c r="B245" s="164" t="s">
         <v>56</v>
       </c>
       <c r="C245" s="63" t="s">
@@ -19278,7 +19270,7 @@
       <c r="A246" s="86" t="s">
         <v>1012</v>
       </c>
-      <c r="B246" s="165" t="s">
+      <c r="B246" s="164" t="s">
         <v>70</v>
       </c>
       <c r="C246" s="63" t="s">
@@ -19305,7 +19297,7 @@
       <c r="A247" s="86" t="s">
         <v>1015</v>
       </c>
-      <c r="B247" s="165" t="s">
+      <c r="B247" s="164" t="s">
         <v>77</v>
       </c>
       <c r="C247" s="63" t="s">
@@ -19332,7 +19324,7 @@
       <c r="A248" s="86" t="s">
         <v>1018</v>
       </c>
-      <c r="B248" s="165" t="s">
+      <c r="B248" s="164" t="s">
         <v>91</v>
       </c>
       <c r="C248" s="63" t="s">
@@ -19359,7 +19351,7 @@
       <c r="A249" s="86" t="s">
         <v>1021</v>
       </c>
-      <c r="B249" s="165" t="s">
+      <c r="B249" s="164" t="s">
         <v>98</v>
       </c>
       <c r="C249" s="63" t="s">
@@ -19386,7 +19378,7 @@
       <c r="A250" s="86" t="s">
         <v>1024</v>
       </c>
-      <c r="B250" s="165" t="s">
+      <c r="B250" s="164" t="s">
         <v>118</v>
       </c>
       <c r="C250" s="66" t="s">
@@ -19413,7 +19405,7 @@
       <c r="A251" s="86" t="s">
         <v>1026</v>
       </c>
-      <c r="B251" s="165" t="s">
+      <c r="B251" s="164" t="s">
         <v>112</v>
       </c>
       <c r="C251" s="63" t="s">
@@ -19440,7 +19432,7 @@
       <c r="A252" s="86" t="s">
         <v>1028</v>
       </c>
-      <c r="B252" s="165" t="s">
+      <c r="B252" s="164" t="s">
         <v>836</v>
       </c>
       <c r="C252" s="63" t="s">
@@ -19467,7 +19459,7 @@
       <c r="A253" s="86" t="s">
         <v>1031</v>
       </c>
-      <c r="B253" s="165" t="s">
+      <c r="B253" s="164" t="s">
         <v>125</v>
       </c>
       <c r="C253" s="63" t="s">
@@ -19491,26 +19483,26 @@
       <c r="K253" s="7"/>
     </row>
     <row r="254">
-      <c r="A254" s="143" t="s">
+      <c r="A254" s="142" t="s">
         <v>1033</v>
       </c>
       <c r="B254" s="62" t="s">
         <v>1034</v>
       </c>
-      <c r="C254" s="168" t="s">
+      <c r="C254" s="167" t="s">
         <v>1035</v>
       </c>
-      <c r="D254" s="168" t="s">
+      <c r="D254" s="167" t="s">
         <v>1036</v>
       </c>
-      <c r="E254" s="169" t="s">
+      <c r="E254" s="168" t="s">
         <v>1037</v>
       </c>
-      <c r="F254" s="169"/>
-      <c r="G254" s="170" t="s">
+      <c r="F254" s="168"/>
+      <c r="G254" s="169" t="s">
         <v>1038</v>
       </c>
-      <c r="H254" s="170" t="s">
+      <c r="H254" s="169" t="s">
         <v>1039</v>
       </c>
       <c r="I254" s="7"/>
@@ -19518,64 +19510,64 @@
       <c r="K254" s="7"/>
     </row>
     <row r="255">
-      <c r="A255" s="171" t="s">
+      <c r="A255" s="170" t="s">
         <v>1040</v>
       </c>
-      <c r="B255" s="172" t="s">
+      <c r="B255" s="171" t="s">
         <v>1041</v>
       </c>
-      <c r="C255" s="173"/>
-      <c r="D255" s="173"/>
-      <c r="E255" s="173"/>
-      <c r="F255" s="173"/>
-      <c r="G255" s="173"/>
-      <c r="H255" s="173"/>
+      <c r="C255" s="172"/>
+      <c r="D255" s="172"/>
+      <c r="E255" s="172"/>
+      <c r="F255" s="172"/>
+      <c r="G255" s="172"/>
+      <c r="H255" s="172"/>
       <c r="I255" s="7"/>
       <c r="J255" s="7"/>
       <c r="K255" s="7"/>
     </row>
     <row r="256">
-      <c r="A256" s="171" t="s">
+      <c r="A256" s="170" t="s">
         <v>1042</v>
       </c>
-      <c r="B256" s="172" t="s">
+      <c r="B256" s="171" t="s">
         <v>1043</v>
       </c>
-      <c r="C256" s="174" t="s">
+      <c r="C256" s="173" t="s">
         <v>739</v>
       </c>
-      <c r="D256" s="173"/>
-      <c r="E256" s="173" t="s">
+      <c r="D256" s="172"/>
+      <c r="E256" s="172" t="s">
         <v>1044</v>
       </c>
-      <c r="F256" s="173"/>
-      <c r="G256" s="173"/>
-      <c r="H256" s="173"/>
+      <c r="F256" s="172"/>
+      <c r="G256" s="172"/>
+      <c r="H256" s="172"/>
       <c r="I256" s="7"/>
       <c r="J256" s="7"/>
       <c r="K256" s="7"/>
     </row>
     <row r="257">
-      <c r="A257" s="171" t="s">
+      <c r="A257" s="170" t="s">
         <v>1045</v>
       </c>
-      <c r="B257" s="172" t="s">
+      <c r="B257" s="171" t="s">
         <v>1046</v>
       </c>
-      <c r="C257" s="173" t="s">
+      <c r="C257" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D257" s="173" t="s">
+      <c r="D257" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E257" s="173" t="s">
+      <c r="E257" s="172" t="s">
         <v>1049</v>
       </c>
-      <c r="F257" s="173"/>
-      <c r="G257" s="173" t="s">
+      <c r="F257" s="172"/>
+      <c r="G257" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H257" s="175" t="s">
+      <c r="H257" s="174" t="s">
         <v>1051</v>
       </c>
       <c r="I257" s="7"/>
@@ -19583,26 +19575,26 @@
       <c r="K257" s="7"/>
     </row>
     <row r="258">
-      <c r="A258" s="171" t="s">
+      <c r="A258" s="170" t="s">
         <v>1052</v>
       </c>
-      <c r="B258" s="172" t="s">
+      <c r="B258" s="171" t="s">
         <v>1053</v>
       </c>
-      <c r="C258" s="173" t="s">
+      <c r="C258" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D258" s="173" t="s">
+      <c r="D258" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E258" s="173" t="s">
+      <c r="E258" s="172" t="s">
         <v>1054</v>
       </c>
-      <c r="F258" s="173"/>
-      <c r="G258" s="173" t="s">
+      <c r="F258" s="172"/>
+      <c r="G258" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H258" s="175" t="s">
+      <c r="H258" s="174" t="s">
         <v>1055</v>
       </c>
       <c r="I258" s="7"/>
@@ -19610,43 +19602,43 @@
       <c r="K258" s="7"/>
     </row>
     <row r="259">
-      <c r="A259" s="171" t="s">
+      <c r="A259" s="170" t="s">
         <v>1056</v>
       </c>
-      <c r="B259" s="172" t="s">
+      <c r="B259" s="171" t="s">
         <v>1057</v>
       </c>
-      <c r="C259" s="173"/>
-      <c r="D259" s="173"/>
-      <c r="E259" s="173"/>
-      <c r="F259" s="173"/>
-      <c r="G259" s="173"/>
-      <c r="H259" s="173"/>
+      <c r="C259" s="172"/>
+      <c r="D259" s="172"/>
+      <c r="E259" s="172"/>
+      <c r="F259" s="172"/>
+      <c r="G259" s="172"/>
+      <c r="H259" s="172"/>
       <c r="I259" s="7"/>
       <c r="J259" s="7"/>
       <c r="K259" s="7"/>
     </row>
     <row r="260">
-      <c r="A260" s="171" t="s">
+      <c r="A260" s="170" t="s">
         <v>1058</v>
       </c>
-      <c r="B260" s="172" t="s">
+      <c r="B260" s="171" t="s">
         <v>1059</v>
       </c>
-      <c r="C260" s="173" t="s">
+      <c r="C260" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D260" s="173" t="s">
+      <c r="D260" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E260" s="173" t="s">
+      <c r="E260" s="172" t="s">
         <v>1060</v>
       </c>
-      <c r="F260" s="173"/>
-      <c r="G260" s="173" t="s">
+      <c r="F260" s="172"/>
+      <c r="G260" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H260" s="175" t="s">
+      <c r="H260" s="174" t="s">
         <v>1061</v>
       </c>
       <c r="I260" s="7"/>
@@ -19654,26 +19646,26 @@
       <c r="K260" s="7"/>
     </row>
     <row r="261">
-      <c r="A261" s="171" t="s">
+      <c r="A261" s="170" t="s">
         <v>1062</v>
       </c>
-      <c r="B261" s="172" t="s">
+      <c r="B261" s="171" t="s">
         <v>1063</v>
       </c>
-      <c r="C261" s="173" t="s">
+      <c r="C261" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D261" s="173" t="s">
+      <c r="D261" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E261" s="173" t="s">
+      <c r="E261" s="172" t="s">
         <v>1064</v>
       </c>
-      <c r="F261" s="173"/>
-      <c r="G261" s="173" t="s">
+      <c r="F261" s="172"/>
+      <c r="G261" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H261" s="175" t="s">
+      <c r="H261" s="174" t="s">
         <v>1065</v>
       </c>
       <c r="I261" s="7"/>
@@ -19681,26 +19673,26 @@
       <c r="K261" s="7"/>
     </row>
     <row r="262">
-      <c r="A262" s="171" t="s">
+      <c r="A262" s="170" t="s">
         <v>1066</v>
       </c>
-      <c r="B262" s="172" t="s">
+      <c r="B262" s="171" t="s">
         <v>1067</v>
       </c>
-      <c r="C262" s="173" t="s">
+      <c r="C262" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D262" s="173" t="s">
+      <c r="D262" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E262" s="173" t="s">
+      <c r="E262" s="172" t="s">
         <v>1068</v>
       </c>
-      <c r="F262" s="173"/>
-      <c r="G262" s="173" t="s">
+      <c r="F262" s="172"/>
+      <c r="G262" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H262" s="175" t="s">
+      <c r="H262" s="174" t="s">
         <v>1069</v>
       </c>
       <c r="I262" s="7"/>
@@ -19708,26 +19700,26 @@
       <c r="K262" s="7"/>
     </row>
     <row r="263">
-      <c r="A263" s="171" t="s">
+      <c r="A263" s="170" t="s">
         <v>1070</v>
       </c>
-      <c r="B263" s="172" t="s">
+      <c r="B263" s="171" t="s">
         <v>1071</v>
       </c>
-      <c r="C263" s="174" t="s">
+      <c r="C263" s="173" t="s">
         <v>1047</v>
       </c>
-      <c r="D263" s="173" t="s">
+      <c r="D263" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E263" s="173" t="s">
+      <c r="E263" s="172" t="s">
         <v>1072</v>
       </c>
-      <c r="F263" s="173"/>
-      <c r="G263" s="173" t="s">
+      <c r="F263" s="172"/>
+      <c r="G263" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H263" s="175" t="s">
+      <c r="H263" s="174" t="s">
         <v>1073</v>
       </c>
       <c r="I263" s="7"/>
@@ -19735,26 +19727,26 @@
       <c r="K263" s="7"/>
     </row>
     <row r="264">
-      <c r="A264" s="171" t="s">
+      <c r="A264" s="170" t="s">
         <v>1074</v>
       </c>
-      <c r="B264" s="172" t="s">
+      <c r="B264" s="171" t="s">
         <v>1075</v>
       </c>
-      <c r="C264" s="174" t="s">
+      <c r="C264" s="173" t="s">
         <v>1047</v>
       </c>
-      <c r="D264" s="173" t="s">
+      <c r="D264" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E264" s="173" t="s">
+      <c r="E264" s="172" t="s">
         <v>1076</v>
       </c>
-      <c r="F264" s="173"/>
-      <c r="G264" s="173" t="s">
+      <c r="F264" s="172"/>
+      <c r="G264" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H264" s="175" t="s">
+      <c r="H264" s="174" t="s">
         <v>1077</v>
       </c>
       <c r="I264" s="7"/>
@@ -19762,45 +19754,45 @@
       <c r="K264" s="7"/>
     </row>
     <row r="265">
-      <c r="A265" s="171" t="s">
+      <c r="A265" s="170" t="s">
         <v>1078</v>
       </c>
-      <c r="B265" s="172" t="s">
+      <c r="B265" s="171" t="s">
         <v>1079</v>
       </c>
-      <c r="C265" s="174" t="s">
+      <c r="C265" s="173" t="s">
         <v>739</v>
       </c>
-      <c r="D265" s="173"/>
-      <c r="E265" s="173"/>
-      <c r="F265" s="173"/>
-      <c r="G265" s="173"/>
-      <c r="H265" s="173"/>
+      <c r="D265" s="172"/>
+      <c r="E265" s="172"/>
+      <c r="F265" s="172"/>
+      <c r="G265" s="172"/>
+      <c r="H265" s="172"/>
       <c r="I265" s="7"/>
       <c r="J265" s="7"/>
       <c r="K265" s="7"/>
     </row>
     <row r="266">
-      <c r="A266" s="171" t="s">
+      <c r="A266" s="170" t="s">
         <v>1080</v>
       </c>
-      <c r="B266" s="172" t="s">
+      <c r="B266" s="171" t="s">
         <v>1081</v>
       </c>
-      <c r="C266" s="173" t="s">
+      <c r="C266" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D266" s="173" t="s">
+      <c r="D266" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E266" s="173" t="s">
+      <c r="E266" s="172" t="s">
         <v>1082</v>
       </c>
-      <c r="F266" s="173"/>
-      <c r="G266" s="173" t="s">
+      <c r="F266" s="172"/>
+      <c r="G266" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H266" s="175" t="s">
+      <c r="H266" s="174" t="s">
         <v>1083</v>
       </c>
       <c r="I266" s="7"/>
@@ -19808,26 +19800,26 @@
       <c r="K266" s="7"/>
     </row>
     <row r="267">
-      <c r="A267" s="171" t="s">
+      <c r="A267" s="170" t="s">
         <v>1084</v>
       </c>
-      <c r="B267" s="172" t="s">
+      <c r="B267" s="171" t="s">
         <v>1085</v>
       </c>
-      <c r="C267" s="173" t="s">
+      <c r="C267" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D267" s="173" t="s">
+      <c r="D267" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E267" s="173" t="s">
+      <c r="E267" s="172" t="s">
         <v>1086</v>
       </c>
-      <c r="F267" s="173"/>
-      <c r="G267" s="173" t="s">
+      <c r="F267" s="172"/>
+      <c r="G267" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H267" s="175" t="s">
+      <c r="H267" s="174" t="s">
         <v>1087</v>
       </c>
       <c r="I267" s="7"/>
@@ -19835,26 +19827,26 @@
       <c r="K267" s="7"/>
     </row>
     <row r="268">
-      <c r="A268" s="171" t="s">
+      <c r="A268" s="170" t="s">
         <v>1088</v>
       </c>
-      <c r="B268" s="172" t="s">
+      <c r="B268" s="171" t="s">
         <v>1089</v>
       </c>
-      <c r="C268" s="173" t="s">
+      <c r="C268" s="172" t="s">
         <v>1047</v>
       </c>
-      <c r="D268" s="173" t="s">
+      <c r="D268" s="172" t="s">
         <v>1048</v>
       </c>
-      <c r="E268" s="173" t="s">
+      <c r="E268" s="172" t="s">
         <v>1090</v>
       </c>
-      <c r="F268" s="173"/>
-      <c r="G268" s="173" t="s">
+      <c r="F268" s="172"/>
+      <c r="G268" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H268" s="175" t="s">
+      <c r="H268" s="174" t="s">
         <v>1091</v>
       </c>
       <c r="I268" s="7"/>
@@ -19862,41 +19854,41 @@
       <c r="K268" s="7"/>
     </row>
     <row r="269">
-      <c r="A269" s="171" t="s">
+      <c r="A269" s="170" t="s">
         <v>1092</v>
       </c>
-      <c r="B269" s="172" t="s">
+      <c r="B269" s="171" t="s">
         <v>1093</v>
       </c>
-      <c r="C269" s="173"/>
-      <c r="D269" s="173"/>
-      <c r="E269" s="173"/>
-      <c r="F269" s="173"/>
-      <c r="G269" s="173"/>
-      <c r="H269" s="173"/>
+      <c r="C269" s="172"/>
+      <c r="D269" s="172"/>
+      <c r="E269" s="172"/>
+      <c r="F269" s="172"/>
+      <c r="G269" s="172"/>
+      <c r="H269" s="172"/>
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
       <c r="K269" s="7"/>
     </row>
     <row r="270">
-      <c r="A270" s="171" t="s">
+      <c r="A270" s="170" t="s">
         <v>1094</v>
       </c>
-      <c r="B270" s="172" t="s">
+      <c r="B270" s="171" t="s">
         <v>1095</v>
       </c>
-      <c r="C270" s="176" t="s">
+      <c r="C270" s="175" t="s">
         <v>607</v>
       </c>
-      <c r="D270" s="173"/>
-      <c r="E270" s="173" t="s">
+      <c r="D270" s="172"/>
+      <c r="E270" s="172" t="s">
         <v>1096</v>
       </c>
-      <c r="F270" s="173"/>
-      <c r="G270" s="173" t="s">
+      <c r="F270" s="172"/>
+      <c r="G270" s="172" t="s">
         <v>1050</v>
       </c>
-      <c r="H270" s="175" t="s">
+      <c r="H270" s="174" t="s">
         <v>1097</v>
       </c>
       <c r="I270" s="7"/>
@@ -19904,43 +19896,43 @@
       <c r="K270" s="7"/>
     </row>
     <row r="271">
-      <c r="A271" s="171" t="s">
+      <c r="A271" s="170" t="s">
         <v>1098</v>
       </c>
-      <c r="B271" s="172" t="s">
+      <c r="B271" s="171" t="s">
         <v>1099</v>
       </c>
-      <c r="C271" s="173"/>
-      <c r="D271" s="173"/>
-      <c r="E271" s="173"/>
-      <c r="F271" s="173"/>
-      <c r="G271" s="173"/>
-      <c r="H271" s="173"/>
+      <c r="C271" s="172"/>
+      <c r="D271" s="172"/>
+      <c r="E271" s="172"/>
+      <c r="F271" s="172"/>
+      <c r="G271" s="172"/>
+      <c r="H271" s="172"/>
       <c r="I271" s="7"/>
       <c r="J271" s="7"/>
       <c r="K271" s="7"/>
     </row>
     <row r="272">
-      <c r="A272" s="171" t="s">
+      <c r="A272" s="170" t="s">
         <v>1100</v>
       </c>
-      <c r="B272" s="172" t="s">
+      <c r="B272" s="171" t="s">
         <v>1101</v>
       </c>
-      <c r="C272" s="174" t="s">
+      <c r="C272" s="173" t="s">
         <v>1102</v>
       </c>
-      <c r="D272" s="173" t="s">
+      <c r="D272" s="172" t="s">
         <v>1103</v>
       </c>
-      <c r="E272" s="177" t="s">
+      <c r="E272" s="176" t="s">
         <v>1104</v>
       </c>
-      <c r="F272" s="173"/>
-      <c r="G272" s="173" t="s">
+      <c r="F272" s="172"/>
+      <c r="G272" s="172" t="s">
         <v>1105</v>
       </c>
-      <c r="H272" s="178" t="s">
+      <c r="H272" s="177" t="s">
         <v>1106</v>
       </c>
       <c r="I272" s="7"/>
@@ -19948,7 +19940,7 @@
       <c r="K272" s="7"/>
     </row>
     <row r="273">
-      <c r="A273" s="179"/>
+      <c r="A273" s="178"/>
       <c r="B273" s="29"/>
       <c r="D273" s="29"/>
       <c r="E273" s="29"/>
@@ -19959,7 +19951,7 @@
       <c r="J273" s="29"/>
     </row>
     <row r="274">
-      <c r="A274" s="179"/>
+      <c r="A274" s="178"/>
       <c r="B274" s="29"/>
       <c r="D274" s="29"/>
       <c r="E274" s="29"/>
@@ -19970,7 +19962,7 @@
       <c r="J274" s="29"/>
     </row>
     <row r="275">
-      <c r="A275" s="179"/>
+      <c r="A275" s="178"/>
       <c r="B275" s="29"/>
       <c r="D275" s="29"/>
       <c r="E275" s="29"/>
@@ -19981,7 +19973,7 @@
       <c r="J275" s="29"/>
     </row>
     <row r="276">
-      <c r="A276" s="179"/>
+      <c r="A276" s="178"/>
       <c r="B276" s="29"/>
       <c r="D276" s="29"/>
       <c r="E276" s="29"/>
@@ -19992,7 +19984,7 @@
       <c r="J276" s="29"/>
     </row>
     <row r="277">
-      <c r="A277" s="179"/>
+      <c r="A277" s="178"/>
       <c r="B277" s="29"/>
       <c r="D277" s="29"/>
       <c r="E277" s="29"/>
@@ -20003,7 +19995,7 @@
       <c r="J277" s="29"/>
     </row>
     <row r="278">
-      <c r="A278" s="179"/>
+      <c r="A278" s="178"/>
       <c r="B278" s="29"/>
       <c r="D278" s="29"/>
       <c r="E278" s="29"/>
@@ -20014,7 +20006,7 @@
       <c r="J278" s="29"/>
     </row>
     <row r="279">
-      <c r="A279" s="179"/>
+      <c r="A279" s="178"/>
       <c r="B279" s="29"/>
       <c r="D279" s="29"/>
       <c r="E279" s="29"/>
@@ -20115,27 +20107,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="179" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="180" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="181" t="s">
+      <c r="C1" s="180" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="181" t="s">
+      <c r="D1" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="181" t="s">
+      <c r="E1" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="181" t="s">
+      <c r="F1" s="180" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="155" t="s">
         <v>362</v>
       </c>
       <c r="B2" s="84" t="s">
@@ -20153,7 +20145,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="155" t="s">
         <v>362</v>
       </c>
       <c r="B3" s="84" t="s">
@@ -20171,7 +20163,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="156" t="s">
+      <c r="A4" s="155" t="s">
         <v>1112</v>
       </c>
       <c r="B4" s="84" t="s">
@@ -20217,7 +20209,7 @@
       <c r="B6" s="84" t="s">
         <v>799</v>
       </c>
-      <c r="C6" s="182" t="s">
+      <c r="C6" s="181" t="s">
         <v>800</v>
       </c>
       <c r="D6" s="7"/>
@@ -20268,7 +20260,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="182" t="s">
         <v>1123</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -20276,7 +20268,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="183" t="s">
         <v>1125</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -20284,12 +20276,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="185" t="s">
+      <c r="A4" s="184" t="s">
         <v>1127</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="186" t="s">
+      <c r="A6" s="185" t="s">
         <v>1128</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -20308,53 +20300,53 @@
       <c r="B9" s="21"/>
     </row>
     <row r="10">
-      <c r="A10" s="186" t="s">
+      <c r="A10" s="185" t="s">
         <v>1131</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="186" t="s">
+      <c r="A11" s="185" t="s">
         <v>1132</v>
       </c>
-      <c r="B11" s="187" t="s">
+      <c r="B11" s="186" t="s">
         <v>1133</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="188" t="s">
+      <c r="B12" s="187" t="s">
         <v>1134</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="189"/>
-      <c r="B13" s="190" t="s">
+      <c r="A13" s="188"/>
+      <c r="B13" s="189" t="s">
         <v>1135</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="191" t="s">
+      <c r="B14" s="190" t="s">
         <v>1136</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="192" t="s">
+      <c r="B15" s="191" t="s">
         <v>1137</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="193" t="s">
+      <c r="B16" s="192" t="s">
         <v>1138</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="186"/>
+      <c r="A17" s="185"/>
       <c r="B17" s="29"/>
     </row>
     <row r="18">
-      <c r="A18" s="186" t="s">
+      <c r="A18" s="185" t="s">
         <v>1139</v>
       </c>
-      <c r="B18" s="194" t="s">
+      <c r="B18" s="193" t="s">
         <v>1140</v>
       </c>
     </row>
@@ -20365,10 +20357,10 @@
       <c r="B19" s="70"/>
     </row>
     <row r="21">
-      <c r="A21" s="186" t="s">
+      <c r="A21" s="185" t="s">
         <v>1142</v>
       </c>
-      <c r="B21" s="195" t="s">
+      <c r="B21" s="194" t="s">
         <v>1143</v>
       </c>
     </row>
@@ -20394,57 +20386,57 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="185" t="s">
         <v>1144</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="195" t="s">
         <v>1145</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="196" t="s">
         <v>1146</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="195" t="s">
         <v>1147</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="197" t="s">
+      <c r="A5" s="196" t="s">
         <v>1148</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="196" t="s">
         <v>1149</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="196" t="s">
         <v>1150</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="196" t="s">
+      <c r="A8" s="195" t="s">
         <v>1151</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="197" t="s">
+      <c r="A9" s="196" t="s">
         <v>1152</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="197" t="s">
+      <c r="A10" s="196" t="s">
         <v>1153</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="196" t="s">
         <v>1154</v>
       </c>
     </row>
@@ -20473,12 +20465,12 @@
       <c r="A1" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="B1" s="198" t="s">
+      <c r="B1" s="197" t="s">
         <v>1155</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="197" t="s">
+      <c r="A2" s="196" t="s">
         <v>1156</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -20486,42 +20478,42 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="196" t="s">
         <v>1158</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="197" t="s">
+      <c r="A4" s="196" t="s">
         <v>1159</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="197" t="s">
+      <c r="A5" s="196" t="s">
         <v>1160</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="196" t="s">
         <v>1161</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="196" t="s">
         <v>1162</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="196" t="s">
         <v>1163</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="197" t="s">
+      <c r="A9" s="196" t="s">
         <v>1164</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="197" t="s">
+      <c r="A10" s="196" t="s">
         <v>1165</v>
       </c>
     </row>
@@ -20541,7 +20533,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="187"/>
+      <c r="A1" s="186"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -20565,10 +20557,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="198" t="s">
         <v>1166</v>
       </c>
-      <c r="C1" s="200" t="s">
+      <c r="C1" s="199" t="s">
         <v>1167</v>
       </c>
     </row>
@@ -20652,7 +20644,7 @@
       <c r="C7" s="7" t="s">
         <v>1174</v>
       </c>
-      <c r="D7" s="201" t="s">
+      <c r="D7" s="200" t="s">
         <v>1183</v>
       </c>
     </row>
@@ -20710,10 +20702,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="198" t="s">
         <v>1166</v>
       </c>
-      <c r="C1" s="200" t="s">
+      <c r="C1" s="199" t="s">
         <v>1167</v>
       </c>
     </row>
@@ -20727,7 +20719,7 @@
       <c r="C2" s="2" t="s">
         <v>1170</v>
       </c>
-      <c r="D2" s="198" t="s">
+      <c r="D2" s="197" t="s">
         <v>1171</v>
       </c>
     </row>
@@ -20758,7 +20750,7 @@
       <c r="B5" s="7" t="s">
         <v>1195</v>
       </c>
-      <c r="C5" s="201" t="s">
+      <c r="C5" s="200" t="s">
         <v>1193</v>
       </c>
       <c r="D5" s="7" t="s">

</xml_diff>

<commit_message>
Generated output for F21, F22 and F25 after syncing mappings for all forms o contain the improvements from TX1.2 feedback.
Generated output for F21, F22 and F25 after syncing mappings for all forms o contain the improvements from TX1.2 feedback.
</commit_message>
<xml_diff>
--- a/mappings/package_F22/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F22/transformation/conceptual_mappings.xlsx
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="1269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1280">
   <si>
     <t>Field</t>
   </si>
@@ -167,7 +167,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.2.1</t>
+    <t>4.2.2</t>
   </si>
   <si>
     <r>
@@ -4624,6 +4624,7 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>?this</t>
     </r>
@@ -4631,6 +4632,7 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:isSubjectToProcedureSpecificTerm  /  epo:hasNationalProcedureRules </t>
     </r>
@@ -4638,6 +4640,7 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>?value</t>
     </r>
@@ -4994,7 +4997,6 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t>?this</t>
     </r>
@@ -5002,7 +5004,6 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:hasTitle </t>
     </r>
@@ -5010,7 +5011,6 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t>?value</t>
     </r>
@@ -5018,7 +5018,6 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -5045,28 +5044,24 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>?this</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:includesLotAwardOutcome / epo:hasAwardStatus   </t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>&lt;http://publications.europa.eu/resource/authority/winner-selection-status/selec-w&gt;</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .
 </t>
@@ -5219,6 +5214,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t>?</t>
     </r>
@@ -5226,12 +5222,14 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>this</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:hasContractConclusionDate ?</t>
     </r>
@@ -5239,12 +5237,14 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>value</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -5816,7 +5816,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>?</t>
     </r>
@@ -5824,14 +5823,12 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t>this</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:playedBy / legal:registeredAddress / locn:postCode ?</t>
     </r>
@@ -5839,14 +5836,12 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t>value</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -5933,7 +5928,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t>?this epo:playedBy / epo:hasPrimaryContactPoint / epo:hasInternetAddress ?</t>
     </r>
@@ -5941,14 +5935,12 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
-        <color theme="1"/>
       </rPr>
       <t>value</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -7368,6 +7360,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t>?</t>
     </r>
@@ -7375,12 +7368,14 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>this</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> epo:playedBy / epo:hasLegalName ?</t>
     </r>
@@ -7388,12 +7383,14 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>value</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -7580,6 +7577,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t>?this epo:playedBy / epo:hasPrimaryContactPoint / epo:hasInternetAddress ?</t>
     </r>
@@ -7587,12 +7585,14 @@
       <rPr>
         <rFont val="Arial"/>
         <b/>
+        <color theme="1"/>
       </rPr>
       <t>value</t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> .</t>
     </r>
@@ -8391,13 +8391,46 @@
     <t>ADDRESS_REVIEW_INFO</t>
   </si>
   <si>
+    <t>AgentInRole == CONTRACTING_BODY/ADDRESS_FURTHER_INFO_IDEM</t>
+  </si>
+  <si>
+    <t>epo:ProcurementProcedureInformationProvider</t>
+  </si>
+  <si>
+    <t>ADDRESS_FURTHER_INFO_IDEM</t>
+  </si>
+  <si>
     <t>AgentInRole == CONTRACTING_BODY/ADDRESS_FURTHER_INFO</t>
   </si>
   <si>
-    <t>epo:ProcurementProcedureInformationProvider</t>
-  </si>
-  <si>
     <t>ADDRESS_FURTHER_INFO</t>
+  </si>
+  <si>
+    <t>AgentInRole == CONTRACTING_BODY/ADDRESS_PARTICIPATION_IDEM</t>
+  </si>
+  <si>
+    <t>epo:TenderReceiver</t>
+  </si>
+  <si>
+    <t>ADDRESS_PARTICIPATION_IDEM</t>
+  </si>
+  <si>
+    <t>AgentInRole == CONTRACTING_BODY/ADDRESS_PARTICIPATION</t>
+  </si>
+  <si>
+    <t>ADDRESS_PARTICIPATION</t>
+  </si>
+  <si>
+    <t>AgentInRole == RESULTS/AWARDED_PRIZE</t>
+  </si>
+  <si>
+    <t>AWARDED_PRIZE</t>
+  </si>
+  <si>
+    <t>AgentInRole == RESULTS/AWARDED_PRIZE/WINNERS/WINNER</t>
+  </si>
+  <si>
+    <t>WINNER</t>
   </si>
   <si>
     <t>is_natural_person == True</t>
@@ -8428,7 +8461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="35">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8504,19 +8537,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Sans-serif"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -8546,6 +8569,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <color rgb="FF0000FF"/>
@@ -8564,16 +8592,6 @@
     <font>
       <u/>
       <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -8617,7 +8635,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8730,6 +8748,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -9151,13 +9175,10 @@
     <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -9169,13 +9190,10 @@
     <xf borderId="0" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9190,10 +9208,10 @@
     <xf borderId="6" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -9211,10 +9229,10 @@
     <xf borderId="0" fillId="7" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="14" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -9226,14 +9244,8 @@
     <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -9246,6 +9258,9 @@
     </xf>
     <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -9283,10 +9298,19 @@
     <xf borderId="0" fillId="6" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9294,9 +9318,6 @@
     </xf>
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -9319,19 +9340,13 @@
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9343,13 +9358,13 @@
     <xf quotePrefix="1" borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -9361,16 +9376,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9397,7 +9412,7 @@
     <xf borderId="0" fillId="18" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="10" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -9412,13 +9427,22 @@
     <xf borderId="0" fillId="19" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="20" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="20" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -16842,7 +16866,7 @@
       <c r="G133" s="42" t="s">
         <v>560</v>
       </c>
-      <c r="H133" s="112" t="s">
+      <c r="H133" s="42" t="s">
         <v>561</v>
       </c>
       <c r="I133" s="7"/>
@@ -16867,7 +16891,7 @@
       <c r="G134" s="41" t="s">
         <v>564</v>
       </c>
-      <c r="H134" s="113" t="s">
+      <c r="H134" s="112" t="s">
         <v>565</v>
       </c>
       <c r="I134" s="7"/>
@@ -16924,7 +16948,7 @@
       <c r="A137" s="56" t="s">
         <v>573</v>
       </c>
-      <c r="B137" s="114" t="s">
+      <c r="B137" s="113" t="s">
         <v>574</v>
       </c>
       <c r="C137" s="100"/>
@@ -16988,16 +17012,16 @@
       <c r="K139" s="7"/>
     </row>
     <row r="140">
-      <c r="A140" s="115" t="s">
+      <c r="A140" s="114" t="s">
         <v>580</v>
       </c>
       <c r="B140" s="70" t="s">
         <v>581</v>
       </c>
-      <c r="C140" s="116" t="s">
+      <c r="C140" s="115" t="s">
         <v>582</v>
       </c>
-      <c r="D140" s="117" t="s">
+      <c r="D140" s="116" t="s">
         <v>583</v>
       </c>
       <c r="E140" s="51" t="s">
@@ -17007,7 +17031,7 @@
       <c r="G140" s="51" t="s">
         <v>585</v>
       </c>
-      <c r="H140" s="118" t="s">
+      <c r="H140" s="52" t="s">
         <v>588</v>
       </c>
       <c r="I140" s="7"/>
@@ -17034,7 +17058,7 @@
       <c r="G141" s="51" t="s">
         <v>594</v>
       </c>
-      <c r="H141" s="119" t="s">
+      <c r="H141" s="117" t="s">
         <v>595</v>
       </c>
       <c r="I141" s="7"/>
@@ -17061,7 +17085,7 @@
       <c r="G142" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="H142" s="120" t="s">
+      <c r="H142" s="118" t="s">
         <v>601</v>
       </c>
       <c r="I142" s="7"/>
@@ -17126,7 +17150,7 @@
       <c r="B146" s="57" t="s">
         <v>609</v>
       </c>
-      <c r="C146" s="121" t="s">
+      <c r="C146" s="119" t="s">
         <v>610</v>
       </c>
       <c r="D146" s="64"/>
@@ -17153,7 +17177,7 @@
       </c>
       <c r="C147" s="64"/>
       <c r="D147" s="64"/>
-      <c r="E147" s="122"/>
+      <c r="E147" s="120"/>
       <c r="F147" s="38"/>
       <c r="G147" s="51"/>
       <c r="H147" s="51"/>
@@ -17171,8 +17195,8 @@
       <c r="C148" s="64" t="s">
         <v>618</v>
       </c>
-      <c r="D148" s="123"/>
-      <c r="E148" s="124" t="s">
+      <c r="D148" s="121"/>
+      <c r="E148" s="122" t="s">
         <v>619</v>
       </c>
       <c r="F148" s="38" t="s">
@@ -17181,7 +17205,7 @@
       <c r="G148" s="51" t="s">
         <v>621</v>
       </c>
-      <c r="H148" s="125" t="s">
+      <c r="H148" s="123" t="s">
         <v>622</v>
       </c>
       <c r="I148" s="7"/>
@@ -17199,7 +17223,7 @@
         <v>625</v>
       </c>
       <c r="D149" s="64"/>
-      <c r="E149" s="122" t="s">
+      <c r="E149" s="120" t="s">
         <v>626</v>
       </c>
       <c r="F149" s="38" t="s">
@@ -17208,7 +17232,7 @@
       <c r="G149" s="51" t="s">
         <v>627</v>
       </c>
-      <c r="H149" s="125" t="s">
+      <c r="H149" s="123" t="s">
         <v>628</v>
       </c>
       <c r="I149" s="7"/>
@@ -17225,8 +17249,8 @@
       <c r="C150" s="64" t="s">
         <v>618</v>
       </c>
-      <c r="D150" s="123"/>
-      <c r="E150" s="124" t="s">
+      <c r="D150" s="121"/>
+      <c r="E150" s="122" t="s">
         <v>631</v>
       </c>
       <c r="F150" s="38" t="s">
@@ -17235,7 +17259,7 @@
       <c r="G150" s="51" t="s">
         <v>621</v>
       </c>
-      <c r="H150" s="126" t="s">
+      <c r="H150" s="124" t="s">
         <v>632</v>
       </c>
       <c r="I150" s="7"/>
@@ -17277,7 +17301,7 @@
       <c r="G152" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="H152" s="113" t="s">
+      <c r="H152" s="112" t="s">
         <v>639</v>
       </c>
       <c r="I152" s="7"/>
@@ -17427,7 +17451,7 @@
       </c>
       <c r="C159" s="64"/>
       <c r="D159" s="64"/>
-      <c r="E159" s="122"/>
+      <c r="E159" s="120"/>
       <c r="F159" s="38"/>
       <c r="G159" s="51"/>
       <c r="H159" s="51"/>
@@ -17445,8 +17469,8 @@
       <c r="C160" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="D160" s="127"/>
-      <c r="E160" s="128" t="s">
+      <c r="D160" s="125"/>
+      <c r="E160" s="126" t="s">
         <v>668</v>
       </c>
       <c r="F160" s="99" t="s">
@@ -17472,8 +17496,8 @@
       <c r="C161" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="D161" s="127"/>
-      <c r="E161" s="129" t="s">
+      <c r="D161" s="125"/>
+      <c r="E161" s="127" t="s">
         <v>668</v>
       </c>
       <c r="F161" s="99" t="s">
@@ -17490,7 +17514,7 @@
       <c r="K161" s="7"/>
     </row>
     <row r="162">
-      <c r="A162" s="130" t="s">
+      <c r="A162" s="128" t="s">
         <v>673</v>
       </c>
       <c r="B162" s="96" t="s">
@@ -17509,7 +17533,7 @@
       <c r="K162" s="7"/>
     </row>
     <row r="163">
-      <c r="A163" s="131" t="s">
+      <c r="A163" s="129" t="s">
         <v>676</v>
       </c>
       <c r="B163" s="40" t="s">
@@ -17562,7 +17586,7 @@
       <c r="G165" s="64" t="s">
         <v>684</v>
       </c>
-      <c r="H165" s="132" t="s">
+      <c r="H165" s="130" t="s">
         <v>685</v>
       </c>
       <c r="I165" s="7"/>
@@ -17589,7 +17613,7 @@
       <c r="G166" s="38" t="s">
         <v>684</v>
       </c>
-      <c r="H166" s="133" t="s">
+      <c r="H166" s="131" t="s">
         <v>689</v>
       </c>
       <c r="I166" s="7"/>
@@ -17643,7 +17667,7 @@
       <c r="G168" s="38" t="s">
         <v>684</v>
       </c>
-      <c r="H168" s="133" t="s">
+      <c r="H168" s="131" t="s">
         <v>697</v>
       </c>
       <c r="I168" s="7"/>
@@ -17728,8 +17752,8 @@
       </c>
       <c r="C172" s="100"/>
       <c r="D172" s="83"/>
-      <c r="E172" s="134"/>
-      <c r="F172" s="135"/>
+      <c r="E172" s="132"/>
+      <c r="F172" s="133"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="7"/>
@@ -17743,18 +17767,18 @@
       <c r="B173" s="57" t="s">
         <v>716</v>
       </c>
-      <c r="C173" s="136" t="s">
+      <c r="C173" s="134" t="s">
         <v>228</v>
       </c>
       <c r="D173" s="85"/>
-      <c r="E173" s="134" t="s">
+      <c r="E173" s="132" t="s">
         <v>717</v>
       </c>
-      <c r="F173" s="135"/>
+      <c r="F173" s="133"/>
       <c r="G173" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="H173" s="137" t="s">
+      <c r="H173" s="34" t="s">
         <v>719</v>
       </c>
       <c r="I173" s="7"/>
@@ -17779,7 +17803,7 @@
       <c r="G174" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="H174" s="113" t="s">
+      <c r="H174" s="112" t="s">
         <v>724</v>
       </c>
       <c r="I174" s="7"/>
@@ -17787,7 +17811,7 @@
       <c r="K174" s="7"/>
     </row>
     <row r="175">
-      <c r="A175" s="131" t="s">
+      <c r="A175" s="129" t="s">
         <v>725</v>
       </c>
       <c r="B175" s="40" t="s">
@@ -17867,7 +17891,7 @@
       <c r="G178" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="H178" s="138" t="s">
+      <c r="H178" s="135" t="s">
         <v>740</v>
       </c>
       <c r="I178" s="7"/>
@@ -17892,7 +17916,7 @@
       <c r="G179" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="H179" s="138" t="s">
+      <c r="H179" s="135" t="s">
         <v>745</v>
       </c>
       <c r="I179" s="7"/>
@@ -17982,7 +18006,7 @@
       <c r="G183" s="38" t="s">
         <v>762</v>
       </c>
-      <c r="H183" s="139" t="s">
+      <c r="H183" s="38" t="s">
         <v>763</v>
       </c>
       <c r="I183" s="7"/>
@@ -17990,7 +18014,7 @@
       <c r="K183" s="7"/>
     </row>
     <row r="184">
-      <c r="A184" s="130" t="s">
+      <c r="A184" s="128" t="s">
         <v>764</v>
       </c>
       <c r="B184" s="36" t="s">
@@ -18015,10 +18039,10 @@
       <c r="K184" s="7"/>
     </row>
     <row r="185">
-      <c r="A185" s="140" t="s">
+      <c r="A185" s="136" t="s">
         <v>764</v>
       </c>
-      <c r="B185" s="141" t="s">
+      <c r="B185" s="137" t="s">
         <v>765</v>
       </c>
       <c r="C185" s="95"/>
@@ -18032,7 +18056,7 @@
       <c r="G185" s="42" t="s">
         <v>770</v>
       </c>
-      <c r="H185" s="142" t="s">
+      <c r="H185" s="138" t="s">
         <v>771</v>
       </c>
       <c r="I185" s="7"/>
@@ -18042,15 +18066,15 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="140" t="s">
+      <c r="A186" s="136" t="s">
         <v>764</v>
       </c>
-      <c r="B186" s="141" t="s">
+      <c r="B186" s="137" t="s">
         <v>765</v>
       </c>
       <c r="C186" s="64"/>
       <c r="D186" s="64"/>
-      <c r="E186" s="143" t="s">
+      <c r="E186" s="139" t="s">
         <v>766</v>
       </c>
       <c r="F186" s="38"/>
@@ -18115,7 +18139,7 @@
       <c r="G188" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="H188" s="106" t="s">
+      <c r="H188" s="140" t="s">
         <v>787</v>
       </c>
       <c r="I188" s="7"/>
@@ -18142,7 +18166,7 @@
       <c r="G189" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="H189" s="41" t="s">
+      <c r="H189" s="135" t="s">
         <v>794</v>
       </c>
       <c r="I189" s="7"/>
@@ -18150,16 +18174,16 @@
       <c r="K189" s="7"/>
     </row>
     <row r="190">
-      <c r="A190" s="144" t="s">
+      <c r="A190" s="141" t="s">
         <v>788</v>
       </c>
-      <c r="B190" s="145" t="s">
+      <c r="B190" s="142" t="s">
         <v>789</v>
       </c>
-      <c r="C190" s="146" t="s">
+      <c r="C190" s="143" t="s">
         <v>790</v>
       </c>
-      <c r="D190" s="117" t="s">
+      <c r="D190" s="116" t="s">
         <v>791</v>
       </c>
       <c r="E190" s="41" t="s">
@@ -18169,7 +18193,7 @@
       <c r="G190" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="H190" s="41" t="s">
+      <c r="H190" s="135" t="s">
         <v>797</v>
       </c>
       <c r="I190" s="7"/>
@@ -18177,13 +18201,13 @@
       <c r="K190" s="7"/>
     </row>
     <row r="191">
-      <c r="A191" s="131" t="s">
+      <c r="A191" s="129" t="s">
         <v>798</v>
       </c>
       <c r="B191" s="40" t="s">
         <v>799</v>
       </c>
-      <c r="C191" s="147" t="s">
+      <c r="C191" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D191" s="64"/>
@@ -18202,7 +18226,7 @@
       <c r="B192" s="49" t="s">
         <v>802</v>
       </c>
-      <c r="C192" s="147" t="s">
+      <c r="C192" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D192" s="64"/>
@@ -18234,7 +18258,7 @@
       <c r="G193" s="38" t="s">
         <v>808</v>
       </c>
-      <c r="H193" s="126" t="s">
+      <c r="H193" s="124" t="s">
         <v>809</v>
       </c>
       <c r="I193" s="7"/>
@@ -18261,7 +18285,7 @@
       <c r="G194" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="H194" s="138" t="s">
+      <c r="H194" s="135" t="s">
         <v>813</v>
       </c>
       <c r="I194" s="7"/>
@@ -18275,7 +18299,7 @@
       <c r="B195" s="57" t="s">
         <v>815</v>
       </c>
-      <c r="C195" s="148" t="s">
+      <c r="C195" s="145" t="s">
         <v>655</v>
       </c>
       <c r="D195" s="64"/>
@@ -18294,13 +18318,13 @@
       <c r="K195" s="7"/>
     </row>
     <row r="196">
-      <c r="A196" s="131" t="s">
+      <c r="A196" s="129" t="s">
         <v>819</v>
       </c>
       <c r="B196" s="40" t="s">
         <v>765</v>
       </c>
-      <c r="C196" s="147" t="s">
+      <c r="C196" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D196" s="64"/>
@@ -18347,7 +18371,7 @@
       <c r="G198" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="H198" s="126" t="s">
+      <c r="H198" s="124" t="s">
         <v>824</v>
       </c>
       <c r="I198" s="7"/>
@@ -18374,7 +18398,7 @@
       <c r="G199" s="41" t="s">
         <v>786</v>
       </c>
-      <c r="H199" s="138" t="s">
+      <c r="H199" s="41" t="s">
         <v>830</v>
       </c>
       <c r="I199" s="7"/>
@@ -18388,12 +18412,12 @@
       <c r="B200" s="49" t="s">
         <v>832</v>
       </c>
-      <c r="C200" s="149"/>
-      <c r="D200" s="149"/>
+      <c r="C200" s="146"/>
+      <c r="D200" s="146"/>
       <c r="E200" s="58" t="s">
         <v>792</v>
       </c>
-      <c r="F200" s="150"/>
+      <c r="F200" s="147"/>
       <c r="G200" s="51" t="s">
         <v>833</v>
       </c>
@@ -18495,8 +18519,8 @@
       <c r="B205" s="57" t="s">
         <v>847</v>
       </c>
-      <c r="C205" s="151"/>
-      <c r="D205" s="151"/>
+      <c r="C205" s="148"/>
+      <c r="D205" s="148"/>
       <c r="E205" s="51" t="s">
         <v>848</v>
       </c>
@@ -18587,7 +18611,7 @@
       <c r="B209" s="57" t="s">
         <v>864</v>
       </c>
-      <c r="C209" s="152" t="s">
+      <c r="C209" s="149" t="s">
         <v>865</v>
       </c>
       <c r="D209" s="64"/>
@@ -18598,7 +18622,7 @@
       <c r="G209" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="H209" s="126" t="s">
+      <c r="H209" s="124" t="s">
         <v>149</v>
       </c>
       <c r="I209" s="7"/>
@@ -18612,7 +18636,7 @@
       <c r="B210" s="49" t="s">
         <v>868</v>
       </c>
-      <c r="C210" s="147" t="s">
+      <c r="C210" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D210" s="64"/>
@@ -18654,8 +18678,8 @@
       <c r="D212" s="100"/>
       <c r="E212" s="100"/>
       <c r="F212" s="100"/>
-      <c r="G212" s="153"/>
-      <c r="H212" s="153"/>
+      <c r="G212" s="150"/>
+      <c r="H212" s="150"/>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
       <c r="K212" s="90" t="s">
@@ -18702,10 +18726,10 @@
       <c r="D214" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="E214" s="154" t="s">
+      <c r="E214" s="151" t="s">
         <v>875</v>
       </c>
-      <c r="F214" s="154"/>
+      <c r="F214" s="151"/>
       <c r="G214" s="47" t="s">
         <v>67</v>
       </c>
@@ -18723,16 +18747,16 @@
       <c r="B215" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="C215" s="155" t="s">
+      <c r="C215" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="D215" s="155" t="s">
+      <c r="D215" s="152" t="s">
         <v>72</v>
       </c>
-      <c r="E215" s="154" t="s">
+      <c r="E215" s="151" t="s">
         <v>878</v>
       </c>
-      <c r="F215" s="154"/>
+      <c r="F215" s="151"/>
       <c r="G215" s="4" t="s">
         <v>74</v>
       </c>
@@ -18750,16 +18774,16 @@
       <c r="B216" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C216" s="155" t="s">
+      <c r="C216" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="D216" s="155" t="s">
+      <c r="D216" s="152" t="s">
         <v>79</v>
       </c>
-      <c r="E216" s="154" t="s">
+      <c r="E216" s="151" t="s">
         <v>881</v>
       </c>
-      <c r="F216" s="154"/>
+      <c r="F216" s="151"/>
       <c r="G216" s="4" t="s">
         <v>74</v>
       </c>
@@ -18777,10 +18801,10 @@
       <c r="B217" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C217" s="155" t="s">
+      <c r="C217" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="D217" s="155" t="s">
+      <c r="D217" s="152" t="s">
         <v>85</v>
       </c>
       <c r="E217" s="82" t="s">
@@ -18806,20 +18830,20 @@
       <c r="B218" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C218" s="155" t="s">
+      <c r="C218" s="152" t="s">
         <v>92</v>
       </c>
-      <c r="D218" s="155" t="s">
+      <c r="D218" s="152" t="s">
         <v>888</v>
       </c>
-      <c r="E218" s="154" t="s">
+      <c r="E218" s="151" t="s">
         <v>889</v>
       </c>
-      <c r="F218" s="154"/>
+      <c r="F218" s="151"/>
       <c r="G218" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H218" s="41" t="s">
+      <c r="H218" s="135" t="s">
         <v>890</v>
       </c>
       <c r="I218" s="7"/>
@@ -18833,16 +18857,16 @@
       <c r="B219" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C219" s="155" t="s">
+      <c r="C219" s="152" t="s">
         <v>99</v>
       </c>
-      <c r="D219" s="155" t="s">
+      <c r="D219" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="E219" s="154" t="s">
+      <c r="E219" s="151" t="s">
         <v>892</v>
       </c>
-      <c r="F219" s="154"/>
+      <c r="F219" s="151"/>
       <c r="G219" s="45" t="s">
         <v>102</v>
       </c>
@@ -18860,16 +18884,16 @@
       <c r="B220" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="C220" s="155" t="s">
+      <c r="C220" s="152" t="s">
         <v>119</v>
       </c>
-      <c r="D220" s="155" t="s">
+      <c r="D220" s="152" t="s">
         <v>120</v>
       </c>
-      <c r="E220" s="154" t="s">
+      <c r="E220" s="151" t="s">
         <v>895</v>
       </c>
-      <c r="F220" s="154"/>
+      <c r="F220" s="151"/>
       <c r="G220" s="51" t="s">
         <v>896</v>
       </c>
@@ -18893,14 +18917,14 @@
       <c r="D221" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="E221" s="154" t="s">
+      <c r="E221" s="151" t="s">
         <v>899</v>
       </c>
-      <c r="F221" s="154"/>
+      <c r="F221" s="151"/>
       <c r="G221" s="66" t="s">
         <v>900</v>
       </c>
-      <c r="H221" s="66" t="s">
+      <c r="H221" s="153" t="s">
         <v>901</v>
       </c>
       <c r="I221" s="7"/>
@@ -18920,14 +18944,14 @@
       <c r="D222" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="E222" s="154" t="s">
+      <c r="E222" s="151" t="s">
         <v>904</v>
       </c>
-      <c r="F222" s="154"/>
+      <c r="F222" s="151"/>
       <c r="G222" s="47" t="s">
         <v>896</v>
       </c>
-      <c r="H222" s="47" t="s">
+      <c r="H222" s="154" t="s">
         <v>905</v>
       </c>
       <c r="I222" s="7"/>
@@ -18947,10 +18971,10 @@
       <c r="D223" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="E223" s="154" t="s">
+      <c r="E223" s="151" t="s">
         <v>907</v>
       </c>
-      <c r="F223" s="154"/>
+      <c r="F223" s="151"/>
       <c r="G223" s="51" t="s">
         <v>900</v>
       </c>
@@ -18974,14 +18998,14 @@
       <c r="D224" s="64" t="s">
         <v>912</v>
       </c>
-      <c r="E224" s="154" t="s">
+      <c r="E224" s="151" t="s">
         <v>913</v>
       </c>
       <c r="F224" s="82"/>
       <c r="G224" s="7" t="s">
         <v>914</v>
       </c>
-      <c r="H224" s="156" t="s">
+      <c r="H224" s="155" t="s">
         <v>915</v>
       </c>
       <c r="I224" s="7"/>
@@ -18989,18 +19013,18 @@
       <c r="K224" s="7"/>
     </row>
     <row r="225">
-      <c r="A225" s="135"/>
+      <c r="A225" s="133"/>
       <c r="B225" s="7"/>
       <c r="C225" s="64"/>
       <c r="D225" s="64"/>
-      <c r="E225" s="157" t="s">
+      <c r="E225" s="156" t="s">
         <v>913</v>
       </c>
       <c r="F225" s="82"/>
       <c r="G225" s="45" t="s">
         <v>916</v>
       </c>
-      <c r="H225" s="45" t="s">
+      <c r="H225" s="157" t="s">
         <v>917</v>
       </c>
       <c r="I225" s="7"/>
@@ -19014,12 +19038,12 @@
       <c r="B226" s="67" t="s">
         <v>919</v>
       </c>
-      <c r="C226" s="147" t="s">
+      <c r="C226" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D226" s="64"/>
-      <c r="E226" s="155"/>
-      <c r="F226" s="155"/>
+      <c r="E226" s="152"/>
+      <c r="F226" s="152"/>
       <c r="G226" s="7"/>
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
@@ -19035,8 +19059,8 @@
       </c>
       <c r="C227" s="100"/>
       <c r="D227" s="100"/>
-      <c r="E227" s="134"/>
-      <c r="F227" s="134"/>
+      <c r="E227" s="132"/>
+      <c r="F227" s="132"/>
       <c r="G227" s="99"/>
       <c r="H227" s="99"/>
       <c r="I227" s="7"/>
@@ -19102,10 +19126,10 @@
         <v>228</v>
       </c>
       <c r="D230" s="64"/>
-      <c r="E230" s="154" t="s">
+      <c r="E230" s="151" t="s">
         <v>927</v>
       </c>
-      <c r="F230" s="154"/>
+      <c r="F230" s="151"/>
       <c r="G230" s="64" t="s">
         <v>928</v>
       </c>
@@ -19129,10 +19153,10 @@
       <c r="D231" s="64" t="s">
         <v>933</v>
       </c>
-      <c r="E231" s="154" t="s">
+      <c r="E231" s="151" t="s">
         <v>934</v>
       </c>
-      <c r="F231" s="154"/>
+      <c r="F231" s="151"/>
       <c r="G231" s="4" t="s">
         <v>935</v>
       </c>
@@ -19154,10 +19178,10 @@
         <v>228</v>
       </c>
       <c r="D232" s="64"/>
-      <c r="E232" s="154" t="s">
+      <c r="E232" s="151" t="s">
         <v>938</v>
       </c>
-      <c r="F232" s="154"/>
+      <c r="F232" s="151"/>
       <c r="G232" s="4" t="s">
         <v>939</v>
       </c>
@@ -19181,10 +19205,10 @@
       <c r="D233" s="64" t="s">
         <v>456</v>
       </c>
-      <c r="E233" s="154" t="s">
+      <c r="E233" s="151" t="s">
         <v>942</v>
       </c>
-      <c r="F233" s="154"/>
+      <c r="F233" s="151"/>
       <c r="G233" s="38" t="s">
         <v>943</v>
       </c>
@@ -19206,14 +19230,14 @@
         <v>228</v>
       </c>
       <c r="D234" s="64"/>
-      <c r="E234" s="154" t="s">
+      <c r="E234" s="151" t="s">
         <v>946</v>
       </c>
-      <c r="F234" s="154"/>
+      <c r="F234" s="151"/>
       <c r="G234" s="64" t="s">
         <v>947</v>
       </c>
-      <c r="H234" s="160" t="s">
+      <c r="H234" s="153" t="s">
         <v>948</v>
       </c>
       <c r="I234" s="7"/>
@@ -19233,10 +19257,10 @@
       <c r="D235" s="64" t="s">
         <v>462</v>
       </c>
-      <c r="E235" s="154" t="s">
+      <c r="E235" s="151" t="s">
         <v>950</v>
       </c>
-      <c r="F235" s="154"/>
+      <c r="F235" s="151"/>
       <c r="G235" s="64" t="s">
         <v>943</v>
       </c>
@@ -19258,7 +19282,7 @@
         <v>228</v>
       </c>
       <c r="D236" s="64"/>
-      <c r="E236" s="161" t="s">
+      <c r="E236" s="160" t="s">
         <v>946</v>
       </c>
       <c r="F236" s="66"/>
@@ -19279,7 +19303,7 @@
       <c r="B237" s="67" t="s">
         <v>955</v>
       </c>
-      <c r="C237" s="147" t="s">
+      <c r="C237" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D237" s="64"/>
@@ -19311,7 +19335,7 @@
       <c r="G238" s="66" t="s">
         <v>961</v>
       </c>
-      <c r="H238" s="162" t="s">
+      <c r="H238" s="161" t="s">
         <v>962</v>
       </c>
       <c r="I238" s="7"/>
@@ -19442,10 +19466,10 @@
       <c r="K243" s="7"/>
     </row>
     <row r="244">
-      <c r="A244" s="130" t="s">
+      <c r="A244" s="128" t="s">
         <v>989</v>
       </c>
-      <c r="B244" s="163" t="s">
+      <c r="B244" s="162" t="s">
         <v>990</v>
       </c>
       <c r="C244" s="7"/>
@@ -19467,8 +19491,8 @@
       </c>
       <c r="C245" s="100"/>
       <c r="D245" s="85"/>
-      <c r="E245" s="134"/>
-      <c r="F245" s="155"/>
+      <c r="E245" s="132"/>
+      <c r="F245" s="152"/>
       <c r="G245" s="66"/>
       <c r="H245" s="66"/>
       <c r="I245" s="7"/>
@@ -19486,10 +19510,10 @@
         <v>995</v>
       </c>
       <c r="D246" s="85"/>
-      <c r="E246" s="134" t="s">
+      <c r="E246" s="132" t="s">
         <v>996</v>
       </c>
-      <c r="F246" s="155"/>
+      <c r="F246" s="152"/>
       <c r="G246" s="7" t="s">
         <v>997</v>
       </c>
@@ -19511,10 +19535,10 @@
         <v>1001</v>
       </c>
       <c r="D247" s="85"/>
-      <c r="E247" s="134" t="s">
+      <c r="E247" s="132" t="s">
         <v>1002</v>
       </c>
-      <c r="F247" s="155"/>
+      <c r="F247" s="152"/>
       <c r="G247" s="7" t="s">
         <v>997</v>
       </c>
@@ -19536,10 +19560,10 @@
         <v>1006</v>
       </c>
       <c r="D248" s="85"/>
-      <c r="E248" s="134" t="s">
+      <c r="E248" s="132" t="s">
         <v>1007</v>
       </c>
-      <c r="F248" s="155"/>
+      <c r="F248" s="152"/>
       <c r="G248" s="7" t="s">
         <v>997</v>
       </c>
@@ -19551,7 +19575,7 @@
       <c r="K248" s="7"/>
     </row>
     <row r="249">
-      <c r="A249" s="131" t="s">
+      <c r="A249" s="129" t="s">
         <v>1009</v>
       </c>
       <c r="B249" s="63" t="s">
@@ -19563,14 +19587,14 @@
       <c r="D249" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="E249" s="154" t="s">
+      <c r="E249" s="151" t="s">
         <v>1010</v>
       </c>
-      <c r="F249" s="154"/>
-      <c r="G249" s="164" t="s">
+      <c r="F249" s="151"/>
+      <c r="G249" s="163" t="s">
         <v>358</v>
       </c>
-      <c r="H249" s="165" t="s">
+      <c r="H249" s="164" t="s">
         <v>1011</v>
       </c>
       <c r="I249" s="7"/>
@@ -19578,18 +19602,18 @@
       <c r="K249" s="7"/>
     </row>
     <row r="250">
-      <c r="A250" s="131" t="s">
+      <c r="A250" s="129" t="s">
         <v>1012</v>
       </c>
       <c r="B250" s="63" t="s">
         <v>1013</v>
       </c>
-      <c r="C250" s="147" t="s">
+      <c r="C250" s="144" t="s">
         <v>800</v>
       </c>
       <c r="D250" s="7"/>
-      <c r="E250" s="155"/>
-      <c r="F250" s="155"/>
+      <c r="E250" s="152"/>
+      <c r="F250" s="152"/>
       <c r="G250" s="7"/>
       <c r="H250" s="7"/>
       <c r="I250" s="7"/>
@@ -19603,7 +19627,7 @@
       <c r="B251" s="67" t="s">
         <v>1015</v>
       </c>
-      <c r="C251" s="166" t="s">
+      <c r="C251" s="165" t="s">
         <v>800</v>
       </c>
       <c r="D251" s="7"/>
@@ -19776,7 +19800,7 @@
       <c r="G257" s="66" t="s">
         <v>896</v>
       </c>
-      <c r="H257" s="160" t="s">
+      <c r="H257" s="153" t="s">
         <v>897</v>
       </c>
       <c r="I257" s="7"/>
@@ -19803,7 +19827,7 @@
       <c r="G258" s="66" t="s">
         <v>900</v>
       </c>
-      <c r="H258" s="160" t="s">
+      <c r="H258" s="153" t="s">
         <v>901</v>
       </c>
       <c r="I258" s="7"/>
@@ -19871,10 +19895,10 @@
       <c r="B261" s="67" t="s">
         <v>1043</v>
       </c>
-      <c r="C261" s="166" t="s">
+      <c r="C261" s="165" t="s">
         <v>800</v>
       </c>
-      <c r="D261" s="167"/>
+      <c r="D261" s="166"/>
       <c r="E261" s="90" t="s">
         <v>1044</v>
       </c>
@@ -19909,7 +19933,7 @@
       <c r="G262" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="H262" s="168" t="s">
+      <c r="H262" s="167" t="s">
         <v>1048</v>
       </c>
       <c r="I262" s="7"/>
@@ -19936,7 +19960,7 @@
       <c r="G263" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="H263" s="168" t="s">
+      <c r="H263" s="167" t="s">
         <v>1051</v>
       </c>
       <c r="I263" s="7"/>
@@ -19990,7 +20014,7 @@
       <c r="G265" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="H265" s="168" t="s">
+      <c r="H265" s="167" t="s">
         <v>1057</v>
       </c>
       <c r="I265" s="7"/>
@@ -20017,7 +20041,7 @@
       <c r="G266" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="H266" s="168" t="s">
+      <c r="H266" s="167" t="s">
         <v>1060</v>
       </c>
       <c r="I266" s="7"/>
@@ -20044,7 +20068,7 @@
       <c r="G267" s="66" t="s">
         <v>896</v>
       </c>
-      <c r="H267" s="160" t="s">
+      <c r="H267" s="66" t="s">
         <v>897</v>
       </c>
       <c r="I267" s="7"/>
@@ -20125,7 +20149,7 @@
       <c r="G270" s="66" t="s">
         <v>900</v>
       </c>
-      <c r="H270" s="160" t="s">
+      <c r="H270" s="66" t="s">
         <v>908</v>
       </c>
       <c r="I270" s="7"/>
@@ -20149,10 +20173,10 @@
         <v>1074</v>
       </c>
       <c r="F271" s="66"/>
-      <c r="G271" s="164" t="s">
+      <c r="G271" s="163" t="s">
         <v>1075</v>
       </c>
-      <c r="H271" s="169" t="s">
+      <c r="H271" s="164" t="s">
         <v>1076</v>
       </c>
       <c r="I271" s="7"/>
@@ -20202,7 +20226,7 @@
       <c r="G273" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="H273" s="168" t="s">
+      <c r="H273" s="90" t="s">
         <v>1082</v>
       </c>
       <c r="I273" s="7"/>
@@ -20229,7 +20253,7 @@
       <c r="G274" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="H274" s="168" t="s">
+      <c r="H274" s="167" t="s">
         <v>1085</v>
       </c>
       <c r="I274" s="7"/>
@@ -20256,7 +20280,7 @@
       <c r="G275" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="H275" s="168" t="s">
+      <c r="H275" s="167" t="s">
         <v>1088</v>
       </c>
       <c r="I275" s="7"/>
@@ -20283,7 +20307,7 @@
       <c r="G276" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="H276" s="168" t="s">
+      <c r="H276" s="167" t="s">
         <v>1091</v>
       </c>
       <c r="I276" s="7"/>
@@ -20310,7 +20334,7 @@
       <c r="G277" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="H277" s="160" t="s">
+      <c r="H277" s="153" t="s">
         <v>1094</v>
       </c>
       <c r="I277" s="7"/>
@@ -20364,7 +20388,7 @@
       <c r="G279" s="66" t="s">
         <v>900</v>
       </c>
-      <c r="H279" s="160" t="s">
+      <c r="H279" s="153" t="s">
         <v>901</v>
       </c>
       <c r="I279" s="7"/>
@@ -20391,7 +20415,7 @@
       <c r="G280" s="62" t="s">
         <v>896</v>
       </c>
-      <c r="H280" s="170" t="s">
+      <c r="H280" s="62" t="s">
         <v>1101</v>
       </c>
       <c r="I280" s="7"/>
@@ -20418,7 +20442,7 @@
       <c r="G281" s="66" t="s">
         <v>900</v>
       </c>
-      <c r="H281" s="160" t="s">
+      <c r="H281" s="66" t="s">
         <v>908</v>
       </c>
       <c r="I281" s="7"/>
@@ -20426,26 +20450,26 @@
       <c r="K281" s="7"/>
     </row>
     <row r="282">
-      <c r="A282" s="131" t="s">
+      <c r="A282" s="129" t="s">
         <v>1104</v>
       </c>
       <c r="B282" s="63" t="s">
         <v>1105</v>
       </c>
-      <c r="C282" s="171" t="s">
+      <c r="C282" s="168" t="s">
         <v>1106</v>
       </c>
-      <c r="D282" s="171" t="s">
+      <c r="D282" s="168" t="s">
         <v>1107</v>
       </c>
-      <c r="E282" s="172" t="s">
+      <c r="E282" s="169" t="s">
         <v>1108</v>
       </c>
-      <c r="F282" s="172"/>
+      <c r="F282" s="169"/>
       <c r="G282" s="90" t="s">
         <v>1109</v>
       </c>
-      <c r="H282" s="173" t="s">
+      <c r="H282" s="170" t="s">
         <v>1110</v>
       </c>
       <c r="I282" s="7"/>
@@ -20453,7 +20477,7 @@
       <c r="K282" s="7"/>
     </row>
     <row r="283">
-      <c r="A283" s="174" t="s">
+      <c r="A283" s="171" t="s">
         <v>1111</v>
       </c>
       <c r="B283" s="100" t="s">
@@ -20470,17 +20494,17 @@
       <c r="K283" s="7"/>
     </row>
     <row r="284">
-      <c r="A284" s="174" t="s">
+      <c r="A284" s="171" t="s">
         <v>1113</v>
       </c>
       <c r="B284" s="100" t="s">
         <v>1114</v>
       </c>
-      <c r="C284" s="175" t="s">
+      <c r="C284" s="172" t="s">
         <v>800</v>
       </c>
       <c r="D284" s="100"/>
-      <c r="E284" s="161" t="s">
+      <c r="E284" s="160" t="s">
         <v>1115</v>
       </c>
       <c r="F284" s="100"/>
@@ -20491,7 +20515,7 @@
       <c r="K284" s="7"/>
     </row>
     <row r="285">
-      <c r="A285" s="174" t="s">
+      <c r="A285" s="171" t="s">
         <v>1116</v>
       </c>
       <c r="B285" s="100" t="s">
@@ -20510,7 +20534,7 @@
       <c r="G285" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H285" s="176" t="s">
+      <c r="H285" s="173" t="s">
         <v>1122</v>
       </c>
       <c r="I285" s="7"/>
@@ -20518,7 +20542,7 @@
       <c r="K285" s="7"/>
     </row>
     <row r="286">
-      <c r="A286" s="174" t="s">
+      <c r="A286" s="171" t="s">
         <v>1123</v>
       </c>
       <c r="B286" s="100" t="s">
@@ -20537,7 +20561,7 @@
       <c r="G286" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H286" s="176" t="s">
+      <c r="H286" s="173" t="s">
         <v>1126</v>
       </c>
       <c r="I286" s="7"/>
@@ -20545,7 +20569,7 @@
       <c r="K286" s="7"/>
     </row>
     <row r="287">
-      <c r="A287" s="174" t="s">
+      <c r="A287" s="171" t="s">
         <v>1127</v>
       </c>
       <c r="B287" s="100" t="s">
@@ -20562,7 +20586,7 @@
       <c r="K287" s="7"/>
     </row>
     <row r="288">
-      <c r="A288" s="174" t="s">
+      <c r="A288" s="171" t="s">
         <v>1129</v>
       </c>
       <c r="B288" s="100" t="s">
@@ -20574,14 +20598,14 @@
       <c r="D288" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E288" s="161" t="s">
+      <c r="E288" s="160" t="s">
         <v>1131</v>
       </c>
       <c r="F288" s="100"/>
       <c r="G288" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H288" s="176" t="s">
+      <c r="H288" s="173" t="s">
         <v>1132</v>
       </c>
       <c r="I288" s="7"/>
@@ -20589,7 +20613,7 @@
       <c r="K288" s="7"/>
     </row>
     <row r="289">
-      <c r="A289" s="174" t="s">
+      <c r="A289" s="171" t="s">
         <v>1133</v>
       </c>
       <c r="B289" s="100" t="s">
@@ -20601,14 +20625,14 @@
       <c r="D289" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E289" s="161" t="s">
+      <c r="E289" s="160" t="s">
         <v>1135</v>
       </c>
       <c r="F289" s="100"/>
       <c r="G289" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H289" s="176" t="s">
+      <c r="H289" s="173" t="s">
         <v>1136</v>
       </c>
       <c r="I289" s="7"/>
@@ -20616,7 +20640,7 @@
       <c r="K289" s="7"/>
     </row>
     <row r="290">
-      <c r="A290" s="174" t="s">
+      <c r="A290" s="171" t="s">
         <v>1137</v>
       </c>
       <c r="B290" s="100" t="s">
@@ -20628,14 +20652,14 @@
       <c r="D290" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E290" s="161" t="s">
+      <c r="E290" s="160" t="s">
         <v>1139</v>
       </c>
       <c r="F290" s="100"/>
       <c r="G290" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H290" s="176" t="s">
+      <c r="H290" s="173" t="s">
         <v>1140</v>
       </c>
       <c r="I290" s="7"/>
@@ -20643,26 +20667,26 @@
       <c r="K290" s="7"/>
     </row>
     <row r="291">
-      <c r="A291" s="174" t="s">
+      <c r="A291" s="171" t="s">
         <v>1141</v>
       </c>
       <c r="B291" s="100" t="s">
         <v>1142</v>
       </c>
-      <c r="C291" s="175" t="s">
+      <c r="C291" s="172" t="s">
         <v>1118</v>
       </c>
       <c r="D291" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E291" s="161" t="s">
+      <c r="E291" s="160" t="s">
         <v>1143</v>
       </c>
       <c r="F291" s="100"/>
       <c r="G291" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H291" s="176" t="s">
+      <c r="H291" s="173" t="s">
         <v>1144</v>
       </c>
       <c r="I291" s="7"/>
@@ -20670,26 +20694,26 @@
       <c r="K291" s="7"/>
     </row>
     <row r="292">
-      <c r="A292" s="174" t="s">
+      <c r="A292" s="171" t="s">
         <v>1145</v>
       </c>
       <c r="B292" s="100" t="s">
         <v>1146</v>
       </c>
-      <c r="C292" s="175" t="s">
+      <c r="C292" s="172" t="s">
         <v>1118</v>
       </c>
       <c r="D292" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E292" s="161" t="s">
+      <c r="E292" s="160" t="s">
         <v>1147</v>
       </c>
       <c r="F292" s="100"/>
       <c r="G292" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H292" s="176" t="s">
+      <c r="H292" s="173" t="s">
         <v>1148</v>
       </c>
       <c r="I292" s="7"/>
@@ -20697,13 +20721,13 @@
       <c r="K292" s="7"/>
     </row>
     <row r="293">
-      <c r="A293" s="174" t="s">
+      <c r="A293" s="171" t="s">
         <v>1149</v>
       </c>
       <c r="B293" s="100" t="s">
         <v>1150</v>
       </c>
-      <c r="C293" s="175" t="s">
+      <c r="C293" s="172" t="s">
         <v>800</v>
       </c>
       <c r="D293" s="100"/>
@@ -20716,7 +20740,7 @@
       <c r="K293" s="7"/>
     </row>
     <row r="294">
-      <c r="A294" s="174" t="s">
+      <c r="A294" s="171" t="s">
         <v>1151</v>
       </c>
       <c r="B294" s="100" t="s">
@@ -20728,14 +20752,14 @@
       <c r="D294" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E294" s="161" t="s">
+      <c r="E294" s="160" t="s">
         <v>1153</v>
       </c>
       <c r="F294" s="100"/>
       <c r="G294" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H294" s="176" t="s">
+      <c r="H294" s="173" t="s">
         <v>1154</v>
       </c>
       <c r="I294" s="7"/>
@@ -20743,7 +20767,7 @@
       <c r="K294" s="7"/>
     </row>
     <row r="295">
-      <c r="A295" s="174" t="s">
+      <c r="A295" s="171" t="s">
         <v>1155</v>
       </c>
       <c r="B295" s="100" t="s">
@@ -20755,14 +20779,14 @@
       <c r="D295" s="100" t="s">
         <v>1119</v>
       </c>
-      <c r="E295" s="161" t="s">
+      <c r="E295" s="160" t="s">
         <v>1157</v>
       </c>
       <c r="F295" s="100"/>
       <c r="G295" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H295" s="176" t="s">
+      <c r="H295" s="173" t="s">
         <v>1158</v>
       </c>
       <c r="I295" s="7"/>
@@ -20770,7 +20794,7 @@
       <c r="K295" s="7"/>
     </row>
     <row r="296">
-      <c r="A296" s="174" t="s">
+      <c r="A296" s="171" t="s">
         <v>1159</v>
       </c>
       <c r="B296" s="100" t="s">
@@ -20789,7 +20813,7 @@
       <c r="G296" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H296" s="176" t="s">
+      <c r="H296" s="173" t="s">
         <v>1162</v>
       </c>
       <c r="I296" s="7"/>
@@ -20797,7 +20821,7 @@
       <c r="K296" s="7"/>
     </row>
     <row r="297">
-      <c r="A297" s="174" t="s">
+      <c r="A297" s="171" t="s">
         <v>1163</v>
       </c>
       <c r="B297" s="100" t="s">
@@ -20814,24 +20838,24 @@
       <c r="K297" s="7"/>
     </row>
     <row r="298">
-      <c r="A298" s="174" t="s">
+      <c r="A298" s="171" t="s">
         <v>1165</v>
       </c>
       <c r="B298" s="100" t="s">
         <v>1166</v>
       </c>
-      <c r="C298" s="177" t="s">
+      <c r="C298" s="174" t="s">
         <v>655</v>
       </c>
       <c r="D298" s="100"/>
-      <c r="E298" s="161" t="s">
+      <c r="E298" s="160" t="s">
         <v>1167</v>
       </c>
       <c r="F298" s="100"/>
       <c r="G298" s="100" t="s">
         <v>1121</v>
       </c>
-      <c r="H298" s="176" t="s">
+      <c r="H298" s="173" t="s">
         <v>1168</v>
       </c>
       <c r="I298" s="7"/>
@@ -20839,7 +20863,7 @@
       <c r="K298" s="7"/>
     </row>
     <row r="299">
-      <c r="A299" s="174" t="s">
+      <c r="A299" s="171" t="s">
         <v>1169</v>
       </c>
       <c r="B299" s="100" t="s">
@@ -20856,19 +20880,19 @@
       <c r="K299" s="7"/>
     </row>
     <row r="300">
-      <c r="A300" s="174" t="s">
+      <c r="A300" s="171" t="s">
         <v>1171</v>
       </c>
       <c r="B300" s="100" t="s">
         <v>1172</v>
       </c>
-      <c r="C300" s="175" t="s">
+      <c r="C300" s="172" t="s">
         <v>1173</v>
       </c>
       <c r="D300" s="100" t="s">
         <v>1174</v>
       </c>
-      <c r="E300" s="178" t="s">
+      <c r="E300" s="175" t="s">
         <v>1175</v>
       </c>
       <c r="F300" s="100"/>
@@ -20913,59 +20937,55 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="H133"/>
-    <hyperlink r:id="rId3" ref="H134"/>
-    <hyperlink r:id="rId4" ref="H140"/>
-    <hyperlink r:id="rId5" ref="H148"/>
-    <hyperlink r:id="rId6" ref="H149"/>
-    <hyperlink r:id="rId7" ref="H150"/>
-    <hyperlink r:id="rId8" ref="H152"/>
-    <hyperlink r:id="rId9" ref="H165"/>
-    <hyperlink r:id="rId10" ref="H166"/>
-    <hyperlink r:id="rId11" ref="H168"/>
-    <hyperlink r:id="rId12" ref="H173"/>
-    <hyperlink r:id="rId13" ref="H174"/>
-    <hyperlink r:id="rId14" ref="H178"/>
-    <hyperlink r:id="rId15" ref="H179"/>
-    <hyperlink r:id="rId16" ref="H183"/>
-    <hyperlink r:id="rId17" ref="H193"/>
-    <hyperlink r:id="rId18" ref="H194"/>
-    <hyperlink r:id="rId19" ref="H198"/>
-    <hyperlink r:id="rId20" ref="H199"/>
-    <hyperlink r:id="rId21" ref="H209"/>
-    <hyperlink r:id="rId22" ref="H224"/>
-    <hyperlink r:id="rId23" ref="H234"/>
-    <hyperlink r:id="rId24" ref="H257"/>
-    <hyperlink r:id="rId25" ref="H258"/>
-    <hyperlink r:id="rId26" ref="H262"/>
-    <hyperlink r:id="rId27" ref="H263"/>
-    <hyperlink r:id="rId28" ref="H265"/>
-    <hyperlink r:id="rId29" ref="H266"/>
-    <hyperlink r:id="rId30" ref="H267"/>
-    <hyperlink r:id="rId31" ref="H270"/>
-    <hyperlink r:id="rId32" ref="H271"/>
-    <hyperlink r:id="rId33" ref="H273"/>
-    <hyperlink r:id="rId34" ref="H274"/>
-    <hyperlink r:id="rId35" ref="H275"/>
-    <hyperlink r:id="rId36" ref="H276"/>
-    <hyperlink r:id="rId37" ref="H277"/>
-    <hyperlink r:id="rId38" ref="H279"/>
-    <hyperlink r:id="rId39" ref="H280"/>
-    <hyperlink r:id="rId40" ref="H281"/>
-    <hyperlink r:id="rId41" ref="H285"/>
-    <hyperlink r:id="rId42" ref="H286"/>
-    <hyperlink r:id="rId43" ref="H288"/>
-    <hyperlink r:id="rId44" ref="H289"/>
-    <hyperlink r:id="rId45" ref="H290"/>
-    <hyperlink r:id="rId46" ref="H291"/>
-    <hyperlink r:id="rId47" ref="H292"/>
-    <hyperlink r:id="rId48" ref="H294"/>
-    <hyperlink r:id="rId49" ref="H295"/>
-    <hyperlink r:id="rId50" ref="H296"/>
-    <hyperlink r:id="rId51" ref="H298"/>
+    <hyperlink r:id="rId2" ref="H134"/>
+    <hyperlink r:id="rId3" ref="H148"/>
+    <hyperlink r:id="rId4" ref="H149"/>
+    <hyperlink r:id="rId5" ref="H150"/>
+    <hyperlink r:id="rId6" ref="H152"/>
+    <hyperlink r:id="rId7" ref="H165"/>
+    <hyperlink r:id="rId8" ref="H166"/>
+    <hyperlink r:id="rId9" ref="H168"/>
+    <hyperlink r:id="rId10" ref="H174"/>
+    <hyperlink r:id="rId11" ref="H178"/>
+    <hyperlink r:id="rId12" ref="H179"/>
+    <hyperlink r:id="rId13" ref="H188"/>
+    <hyperlink r:id="rId14" ref="H189"/>
+    <hyperlink r:id="rId15" ref="H190"/>
+    <hyperlink r:id="rId16" ref="H193"/>
+    <hyperlink r:id="rId17" ref="H194"/>
+    <hyperlink r:id="rId18" ref="H198"/>
+    <hyperlink r:id="rId19" ref="H209"/>
+    <hyperlink r:id="rId20" ref="H218"/>
+    <hyperlink r:id="rId21" ref="H221"/>
+    <hyperlink r:id="rId22" ref="H222"/>
+    <hyperlink r:id="rId23" ref="H224"/>
+    <hyperlink r:id="rId24" ref="H225"/>
+    <hyperlink r:id="rId25" ref="H234"/>
+    <hyperlink r:id="rId26" ref="H257"/>
+    <hyperlink r:id="rId27" ref="H258"/>
+    <hyperlink r:id="rId28" ref="H262"/>
+    <hyperlink r:id="rId29" ref="H263"/>
+    <hyperlink r:id="rId30" ref="H265"/>
+    <hyperlink r:id="rId31" ref="H266"/>
+    <hyperlink r:id="rId32" ref="H274"/>
+    <hyperlink r:id="rId33" ref="H275"/>
+    <hyperlink r:id="rId34" ref="H276"/>
+    <hyperlink r:id="rId35" ref="H277"/>
+    <hyperlink r:id="rId36" ref="H279"/>
+    <hyperlink r:id="rId37" ref="H285"/>
+    <hyperlink r:id="rId38" ref="H286"/>
+    <hyperlink r:id="rId39" ref="H288"/>
+    <hyperlink r:id="rId40" ref="H289"/>
+    <hyperlink r:id="rId41" ref="H290"/>
+    <hyperlink r:id="rId42" ref="H291"/>
+    <hyperlink r:id="rId43" ref="H292"/>
+    <hyperlink r:id="rId44" ref="H294"/>
+    <hyperlink r:id="rId45" ref="H295"/>
+    <hyperlink r:id="rId46" ref="H296"/>
+    <hyperlink r:id="rId47" ref="H298"/>
   </hyperlinks>
-  <drawing r:id="rId52"/>
-  <legacyDrawing r:id="rId53"/>
+  <drawing r:id="rId48"/>
+  <legacyDrawing r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -20987,27 +21007,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="180" t="s">
+      <c r="B1" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="180" t="s">
+      <c r="C1" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="180" t="s">
+      <c r="D1" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="180" t="s">
+      <c r="E1" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="180" t="s">
+      <c r="F1" s="177" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="133" t="s">
         <v>411</v>
       </c>
       <c r="B2" s="90" t="s">
@@ -21025,7 +21045,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="133" t="s">
         <v>411</v>
       </c>
       <c r="B3" s="90" t="s">
@@ -21043,7 +21063,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="135" t="s">
+      <c r="A4" s="133" t="s">
         <v>1183</v>
       </c>
       <c r="B4" s="90" t="s">
@@ -21089,7 +21109,7 @@
       <c r="B6" s="90" t="s">
         <v>864</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="178" t="s">
         <v>865</v>
       </c>
       <c r="D6" s="7"/>
@@ -21140,7 +21160,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="179" t="s">
         <v>1194</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -21148,7 +21168,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="180" t="s">
         <v>1196</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -21156,12 +21176,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="181" t="s">
         <v>1198</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="185" t="s">
+      <c r="A6" s="182" t="s">
         <v>1199</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -21180,53 +21200,53 @@
       <c r="B9" s="21"/>
     </row>
     <row r="10">
-      <c r="A10" s="185" t="s">
+      <c r="A10" s="182" t="s">
         <v>1202</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="185" t="s">
+      <c r="A11" s="182" t="s">
         <v>1203</v>
       </c>
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="183" t="s">
         <v>1204</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="187" t="s">
+      <c r="B12" s="184" t="s">
         <v>1205</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="188"/>
-      <c r="B13" s="189" t="s">
+      <c r="A13" s="185"/>
+      <c r="B13" s="186" t="s">
         <v>1206</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="190" t="s">
+      <c r="B14" s="187" t="s">
         <v>1207</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="191" t="s">
+      <c r="B15" s="188" t="s">
         <v>1208</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="189" t="s">
         <v>1209</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="185"/>
+      <c r="A17" s="182"/>
       <c r="B17" s="29"/>
     </row>
     <row r="18">
-      <c r="A18" s="185" t="s">
+      <c r="A18" s="182" t="s">
         <v>1210</v>
       </c>
-      <c r="B18" s="193" t="s">
+      <c r="B18" s="190" t="s">
         <v>1211</v>
       </c>
     </row>
@@ -21237,10 +21257,10 @@
       <c r="B19" s="84"/>
     </row>
     <row r="21">
-      <c r="A21" s="185" t="s">
+      <c r="A21" s="182" t="s">
         <v>1213</v>
       </c>
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="191" t="s">
         <v>1214</v>
       </c>
     </row>
@@ -21266,57 +21286,57 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="182" t="s">
         <v>1215</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="195" t="s">
+      <c r="A2" s="192" t="s">
         <v>1216</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="193" t="s">
         <v>1217</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="195" t="s">
+      <c r="A4" s="192" t="s">
         <v>1218</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="193" t="s">
         <v>1219</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="193" t="s">
         <v>1220</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="196" t="s">
+      <c r="A7" s="193" t="s">
         <v>1221</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="195" t="s">
+      <c r="A8" s="192" t="s">
         <v>1222</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="196" t="s">
+      <c r="A9" s="193" t="s">
         <v>1223</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="196" t="s">
+      <c r="A10" s="193" t="s">
         <v>1224</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="196" t="s">
+      <c r="A11" s="193" t="s">
         <v>1225</v>
       </c>
     </row>
@@ -21345,12 +21365,12 @@
       <c r="A1" s="1" t="s">
         <v>1215</v>
       </c>
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="194" t="s">
         <v>1226</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="193" t="s">
         <v>1227</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -21358,47 +21378,47 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="193" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="193" t="s">
         <v>1230</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="196" t="s">
+      <c r="A5" s="193" t="s">
         <v>1231</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="196" t="s">
+      <c r="A6" s="193" t="s">
         <v>1232</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="196" t="s">
+      <c r="A7" s="193" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="196" t="s">
+      <c r="A8" s="193" t="s">
         <v>1234</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="196" t="s">
+      <c r="A9" s="193" t="s">
         <v>1235</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="196" t="s">
+      <c r="A10" s="193" t="s">
         <v>1236</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="195" t="s">
         <v>1237</v>
       </c>
     </row>
@@ -21418,7 +21438,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="186"/>
+      <c r="A1" s="183"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -21442,12 +21462,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="196" t="s">
         <v>1238</v>
       </c>
-      <c r="C1" s="200" t="s">
+      <c r="C1" s="197" t="s">
         <v>1239</v>
       </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -21462,12 +21504,34 @@
       <c r="D2" s="2" t="s">
         <v>1243</v>
       </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>1244</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>1245</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -21477,21 +21541,65 @@
         <f t="shared" ref="D3:D4" si="1">RIGHT(A3,LEN(A3) - (FIND(" == ",A3) + 3))</f>
         <v>ADDRESS_CONTRACTING_BODY</v>
       </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>1247</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>1245</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>1246</v>
       </c>
-      <c r="D4" s="19" t="str">
+      <c r="D4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ADDRESS_CONTRACTING_BODY_ADDITIONAL</v>
       </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
@@ -21504,6 +21612,28 @@
         <v>1246</v>
       </c>
       <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -21515,9 +21645,31 @@
       <c r="C6" s="7" t="s">
         <v>1246</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="7" t="s">
         <v>1252</v>
       </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
@@ -21529,9 +21681,31 @@
       <c r="C7" s="7" t="s">
         <v>1246</v>
       </c>
-      <c r="D7" s="201" t="s">
+      <c r="D7" s="198" t="s">
         <v>1255</v>
       </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
@@ -21546,12 +21720,34 @@
       <c r="D8" s="7" t="s">
         <v>1258</v>
       </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="90" t="s">
         <v>1259</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="7" t="s">
         <v>1260</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -21560,6 +21756,208 @@
       <c r="D9" s="7" t="s">
         <v>1261</v>
       </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="90" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="90" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="90" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="199" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B13" s="199" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C13" s="200" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D13" s="200" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E13" s="200"/>
+      <c r="F13" s="200"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="200"/>
+      <c r="I13" s="200"/>
+      <c r="J13" s="200"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="200"/>
+      <c r="M13" s="200"/>
+      <c r="N13" s="200"/>
+      <c r="O13" s="200"/>
+      <c r="P13" s="200"/>
+      <c r="Q13" s="200"/>
+      <c r="R13" s="200"/>
+      <c r="S13" s="200"/>
+      <c r="T13" s="200"/>
+      <c r="U13" s="200"/>
+      <c r="V13" s="200"/>
+      <c r="W13" s="200"/>
+      <c r="X13" s="200"/>
+      <c r="Y13" s="200"/>
+      <c r="Z13" s="200"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="199" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B14" s="199" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C14" s="200" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D14" s="200" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E14" s="200"/>
+      <c r="F14" s="200"/>
+      <c r="G14" s="200"/>
+      <c r="H14" s="200"/>
+      <c r="I14" s="200"/>
+      <c r="J14" s="200"/>
+      <c r="K14" s="200"/>
+      <c r="L14" s="200"/>
+      <c r="M14" s="200"/>
+      <c r="N14" s="200"/>
+      <c r="O14" s="200"/>
+      <c r="P14" s="200"/>
+      <c r="Q14" s="200"/>
+      <c r="R14" s="200"/>
+      <c r="S14" s="200"/>
+      <c r="T14" s="200"/>
+      <c r="U14" s="200"/>
+      <c r="V14" s="200"/>
+      <c r="W14" s="200"/>
+      <c r="X14" s="200"/>
+      <c r="Y14" s="200"/>
+      <c r="Z14" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -21587,10 +21985,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="196" t="s">
         <v>1238</v>
       </c>
-      <c r="C1" s="200" t="s">
+      <c r="C1" s="197" t="s">
         <v>1239</v>
       </c>
     </row>
@@ -21604,42 +22002,42 @@
       <c r="C2" s="2" t="s">
         <v>1242</v>
       </c>
-      <c r="D2" s="197" t="s">
+      <c r="D2" s="194" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1262</v>
+        <v>1273</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1263</v>
+        <v>1274</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>1264</v>
+        <v>1275</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1265</v>
+        <v>1276</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>1266</v>
+        <v>1277</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1267</v>
+        <v>1278</v>
       </c>
       <c r="C5" s="201" t="s">
-        <v>1265</v>
+        <v>1276</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1268</v>
+        <v>1279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>